<commit_message>
Mass properties on Excel finished.
Finished the mass properties in the excel, with the new vertical connectors.
</commit_message>
<xml_diff>
--- a/PoCat3_Thermal_Model_Mass_Properties.xlsx
+++ b/PoCat3_Thermal_Model_Mass_Properties.xlsx
@@ -8,22 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oscar\Documents\GitHub\PoCat-Thermal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F6255F3-D468-42FC-848E-8D2016502917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7ABFF36-B90D-4CA4-9CFE-AA59A1870ACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Materials" sheetId="1" r:id="rId1"/>
     <sheet name="Masses and Volumes" sheetId="7" r:id="rId2"/>
-    <sheet name="Bulks" sheetId="6" r:id="rId3"/>
-    <sheet name="Optical" sheetId="5" r:id="rId4"/>
+    <sheet name="Masses and Volumes New VC" sheetId="8" r:id="rId3"/>
+    <sheet name="Bulks" sheetId="6" r:id="rId4"/>
+    <sheet name="Optical" sheetId="5" r:id="rId5"/>
+    <sheet name="Extra" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="172">
   <si>
     <t>Material</t>
   </si>
@@ -265,9 +267,6 @@
     <t>OCB-COMMS PCB++</t>
   </si>
   <si>
-    <t>Y+ Mag PCB ++</t>
-  </si>
-  <si>
     <t>Top PL PCB</t>
   </si>
   <si>
@@ -277,39 +276,21 @@
     <t>Notes:</t>
   </si>
   <si>
-    <t>Prob ignore</t>
-  </si>
-  <si>
     <t>With VC and components</t>
   </si>
   <si>
     <t>With components</t>
   </si>
   <si>
-    <t>PTFE?</t>
-  </si>
-  <si>
     <t>COMMS Antenna</t>
   </si>
   <si>
     <t>Comms</t>
   </si>
   <si>
-    <t>Prob ignore (Total mass)</t>
-  </si>
-  <si>
-    <t>kg/unit</t>
-  </si>
-  <si>
     <t>ESATAN Volume (m^3)</t>
   </si>
   <si>
-    <t>Have to fix VC</t>
-  </si>
-  <si>
-    <t>in PCB</t>
-  </si>
-  <si>
     <t>Material Density (kg· m^-3)</t>
   </si>
   <si>
@@ -346,18 +327,6 @@
     <t>Mass (kg)</t>
   </si>
   <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>Calculated or Measured</t>
-  </si>
-  <si>
     <t>SD_KS_PX</t>
   </si>
   <si>
@@ -481,9 +450,6 @@
     <t>Vertical Connectors (new)</t>
   </si>
   <si>
-    <t>2.2g (4)</t>
-  </si>
-  <si>
     <t>2.9g (4)</t>
   </si>
   <si>
@@ -523,7 +489,58 @@
     <t>Y mag raw</t>
   </si>
   <si>
-    <t>la unidad</t>
+    <t>Mass (kg/unit)</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>Total mass (kg)</t>
+  </si>
+  <si>
+    <t>Total mass (g)</t>
+  </si>
+  <si>
+    <t>Included</t>
+  </si>
+  <si>
+    <t>Y+ Mag PCB +</t>
+  </si>
+  <si>
+    <t>AOCS PCB+</t>
+  </si>
+  <si>
+    <t>EPS PCB +</t>
+  </si>
+  <si>
+    <t>OCB-COMMS PCB+</t>
+  </si>
+  <si>
+    <t>+ (With components)</t>
+  </si>
+  <si>
+    <t>Inner Connectors</t>
+  </si>
+  <si>
+    <t>Not added (resolution)</t>
+  </si>
+  <si>
+    <t>Not added (included in lats)</t>
+  </si>
+  <si>
+    <t>lateral</t>
+  </si>
+  <si>
+    <t>laterals comps</t>
+  </si>
+  <si>
+    <t>lateral comps solar</t>
+  </si>
+  <si>
+    <t>lateral comps solar thermal</t>
+  </si>
+  <si>
+    <t>Lateral PCB Thermal +</t>
   </si>
 </sst>
 </file>
@@ -655,7 +672,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -710,6 +727,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1523,10 +1557,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D60A6198-9637-4F08-B05D-DA5383A125B7}">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1536,13 +1570,15 @@
     <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" customWidth="1"/>
+    <col min="7" max="7" width="9.21875" customWidth="1"/>
+    <col min="8" max="8" width="14.5546875" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
+    <col min="10" max="10" width="25.44140625" customWidth="1"/>
+    <col min="11" max="11" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>26</v>
       </c>
@@ -1553,38 +1589,41 @@
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>27</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>106</v>
+        <v>154</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>110</v>
+        <v>155</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="I1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
-      <c r="I2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>44</v>
       </c>
@@ -1598,18 +1637,26 @@
         <v>1850</v>
       </c>
       <c r="E3" s="6">
-        <f t="shared" ref="E3:E15" si="0">J3/1000/1000/1000</f>
+        <f t="shared" ref="E3:E15" si="0">L3/1000/1000/1000</f>
         <v>0</v>
       </c>
       <c r="F3" s="6">
         <v>8.3999999999999995E-3</v>
       </c>
-      <c r="G3" t="s">
-        <v>107</v>
-      </c>
-      <c r="H3" s="5"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G3" s="6">
+        <v>1</v>
+      </c>
+      <c r="H3" s="6">
+        <f>F3*G3</f>
+        <v>8.3999999999999995E-3</v>
+      </c>
+      <c r="I3" s="6">
+        <f>H3*1000</f>
+        <v>8.4</v>
+      </c>
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>75</v>
       </c>
@@ -1629,16 +1676,24 @@
       <c r="F4" s="6">
         <v>1.66E-2</v>
       </c>
-      <c r="G4" t="s">
-        <v>107</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G4" s="6">
+        <v>1</v>
+      </c>
+      <c r="H4" s="6">
+        <f t="shared" ref="H4:I37" si="1">F4*G4</f>
+        <v>1.66E-2</v>
+      </c>
+      <c r="I4" s="6">
+        <f t="shared" ref="I4:I39" si="2">H4*1000</f>
+        <v>16.600000000000001</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>80</v>
+        <v>159</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>66</v>
@@ -1656,15 +1711,23 @@
       <c r="F5" s="6">
         <v>6.6E-3</v>
       </c>
-      <c r="G5" t="s">
-        <v>107</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G5" s="6">
+        <v>1</v>
+      </c>
+      <c r="H5" s="6">
+        <f t="shared" si="1"/>
+        <v>6.6E-3</v>
+      </c>
+      <c r="I5" s="6">
+        <f t="shared" si="2"/>
+        <v>6.6</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>77</v>
       </c>
@@ -1684,14 +1747,22 @@
       <c r="F6" s="6">
         <v>1.0199999999999999E-2</v>
       </c>
-      <c r="G6" t="s">
-        <v>107</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G6" s="6">
+        <v>1</v>
+      </c>
+      <c r="H6" s="6">
+        <f t="shared" si="1"/>
+        <v>1.0199999999999999E-2</v>
+      </c>
+      <c r="I6" s="6">
+        <f t="shared" si="2"/>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>78</v>
       </c>
@@ -1711,14 +1782,22 @@
       <c r="F7" s="6">
         <v>9.300000000000001E-3</v>
       </c>
-      <c r="G7" t="s">
-        <v>107</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G7" s="6">
+        <v>1</v>
+      </c>
+      <c r="H7" s="6">
+        <f t="shared" si="1"/>
+        <v>9.300000000000001E-3</v>
+      </c>
+      <c r="I7" s="6">
+        <f t="shared" si="2"/>
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>79</v>
       </c>
@@ -1738,14 +1817,22 @@
       <c r="F8" s="6">
         <v>9.1999999999999998E-3</v>
       </c>
-      <c r="G8" t="s">
-        <v>107</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G8" s="6">
+        <v>1</v>
+      </c>
+      <c r="H8" s="6">
+        <f t="shared" si="1"/>
+        <v>9.1999999999999998E-3</v>
+      </c>
+      <c r="I8" s="6">
+        <f t="shared" si="2"/>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>76</v>
       </c>
@@ -1765,19 +1852,27 @@
       <c r="F9" s="6">
         <v>1.11E-2</v>
       </c>
-      <c r="G9" t="s">
-        <v>108</v>
-      </c>
-      <c r="H9" s="5" t="s">
+      <c r="G9" s="6">
+        <v>4</v>
+      </c>
+      <c r="H9" s="6">
+        <f t="shared" si="1"/>
+        <v>4.4400000000000002E-2</v>
+      </c>
+      <c r="I9" s="6">
+        <f t="shared" si="2"/>
+        <v>44.4</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>89</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>49</v>
@@ -1790,28 +1885,36 @@
       <c r="F10" s="6">
         <v>5.7000000000000002E-3</v>
       </c>
-      <c r="G10" t="s">
-        <v>107</v>
-      </c>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G10" s="6">
+        <v>1</v>
+      </c>
+      <c r="H10" s="6">
+        <f t="shared" si="1"/>
+        <v>5.7000000000000002E-3</v>
+      </c>
+      <c r="I10" s="6">
+        <f t="shared" si="2"/>
+        <v>5.7</v>
+      </c>
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
-      <c r="E11" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="E11" s="6"/>
       <c r="F11" s="6"/>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="5"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>73</v>
@@ -1829,14 +1932,22 @@
       <c r="F12" s="6">
         <v>9.1999999999999998E-3</v>
       </c>
-      <c r="G12" t="s">
-        <v>107</v>
-      </c>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G12" s="6">
+        <v>1</v>
+      </c>
+      <c r="H12" s="6">
+        <f t="shared" si="1"/>
+        <v>9.1999999999999998E-3</v>
+      </c>
+      <c r="I12" s="6">
+        <f t="shared" si="2"/>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>71</v>
@@ -1854,12 +1965,20 @@
       <c r="F13" s="6">
         <v>7.6E-3</v>
       </c>
-      <c r="G13" t="s">
-        <v>107</v>
-      </c>
-      <c r="H13" s="5"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G13" s="6">
+        <v>1</v>
+      </c>
+      <c r="H13" s="6">
+        <f t="shared" si="1"/>
+        <v>7.6E-3</v>
+      </c>
+      <c r="I13" s="6">
+        <f t="shared" si="2"/>
+        <v>7.6</v>
+      </c>
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>46</v>
       </c>
@@ -1879,14 +1998,20 @@
       <c r="F14" s="6">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="G14" t="s">
-        <v>107</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G14" s="6">
+        <v>1</v>
+      </c>
+      <c r="H14" s="6">
+        <f t="shared" si="1"/>
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="I14" s="6">
+        <f t="shared" si="2"/>
+        <v>0.7</v>
+      </c>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>47</v>
       </c>
@@ -1906,17 +2031,25 @@
       <c r="F15" s="6">
         <v>2.4300000000000002E-2</v>
       </c>
-      <c r="G15" t="s">
-        <v>107</v>
-      </c>
-      <c r="H15" s="5"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G15" s="6">
+        <v>1</v>
+      </c>
+      <c r="H15" s="6">
+        <f t="shared" si="1"/>
+        <v>2.4300000000000002E-2</v>
+      </c>
+      <c r="I15" s="6">
+        <f t="shared" si="2"/>
+        <v>24.3</v>
+      </c>
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
-      <c r="H16" s="5"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>42</v>
       </c>
@@ -1924,13 +2057,22 @@
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
       <c r="E17" s="11">
-        <f>J17/1000/1000/1000</f>
+        <f>L17/1000/1000/1000</f>
         <v>0</v>
       </c>
       <c r="F17" s="11"/>
-      <c r="H17" s="5"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G17" s="11"/>
+      <c r="H17" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>43</v>
       </c>
@@ -1944,20 +2086,26 @@
         <v>5316</v>
       </c>
       <c r="E18" s="11">
-        <f>J18/1000/1000/1000</f>
+        <f>L18/1000/1000/1000</f>
         <v>0</v>
       </c>
       <c r="F18" s="11">
         <v>9.5E-4</v>
       </c>
-      <c r="G18" t="s">
-        <v>107</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G18" s="11">
+        <v>5</v>
+      </c>
+      <c r="H18" s="11">
+        <f t="shared" si="1"/>
+        <v>4.7499999999999999E-3</v>
+      </c>
+      <c r="I18" s="11">
+        <f t="shared" si="2"/>
+        <v>4.75</v>
+      </c>
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
         <v>17</v>
       </c>
@@ -1971,37 +2119,48 @@
         <v>2750</v>
       </c>
       <c r="E19" s="11">
-        <f>J19/1000/1000/1000</f>
+        <f>L19/1000/1000/1000</f>
         <v>0</v>
       </c>
       <c r="F19" s="11">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="G19" t="s">
-        <v>107</v>
-      </c>
-      <c r="H19" s="5"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G19" s="11">
+        <v>1</v>
+      </c>
+      <c r="H19" s="11">
+        <f t="shared" si="1"/>
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="I19" s="11">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="J19" s="5"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
-      <c r="H20" s="5"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J20" s="5"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="B21" s="13"/>
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
-      <c r="E21" s="14">
-        <f>J21/1000/1000/1000</f>
-        <v>0</v>
-      </c>
+      <c r="E21" s="14"/>
       <c r="F21" s="14"/>
-      <c r="H21" s="5"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J21" s="5"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
         <v>55</v>
       </c>
@@ -2015,20 +2174,21 @@
         <v>8800</v>
       </c>
       <c r="E22" s="14">
-        <f>J22/1000/1000/1000</f>
-        <v>0</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G22" t="s">
-        <v>109</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+        <f>L22/1000/1000/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="5"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>56</v>
       </c>
@@ -2042,108 +2202,109 @@
         <v>1070</v>
       </c>
       <c r="E23" s="14">
-        <f>J23/1000/1000/1000</f>
-        <v>0</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G23" t="s">
-        <v>109</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B24" s="5"/>
-      <c r="E24" t="s">
-        <v>152</v>
-      </c>
-      <c r="H24" s="5"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="16" t="s">
+        <f>L23/1000/1000/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F23" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J23" s="5"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="15"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14">
+        <v>5.5000000000000003E-4</v>
+      </c>
+      <c r="G24" s="14">
+        <v>14.75</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="J24" s="5"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="J25" s="5"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="16"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17">
-        <f>J25/1000/1000/1000</f>
-        <v>0</v>
-      </c>
-      <c r="F25" s="17"/>
-      <c r="H25" s="5"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="18" t="s">
+      <c r="B26" s="16"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="5"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="B27" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C27" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17">
-        <f>J26/1000/1000/1000</f>
-        <v>0</v>
-      </c>
-      <c r="F26" s="17">
+      <c r="D27" s="17"/>
+      <c r="E27" s="17">
+        <f>L27/1000/1000/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F27" s="17">
         <v>0.03</v>
       </c>
-      <c r="G26" t="s">
-        <v>107</v>
-      </c>
-      <c r="H26" s="5"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="16" t="s">
+      <c r="G27" s="17">
+        <v>1</v>
+      </c>
+      <c r="H27" s="17">
+        <f t="shared" si="1"/>
+        <v>0.03</v>
+      </c>
+      <c r="I27" s="17">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="J27" s="5"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="16"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="H27" s="5"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="18" t="s">
+      <c r="B28" s="16"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="5"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="18" t="s">
         <v>36</v>
-      </c>
-      <c r="B28" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="D28" s="17">
-        <v>8000</v>
-      </c>
-      <c r="E28" s="17">
-        <f>J28/1000/1000/1000</f>
-        <v>0</v>
-      </c>
-      <c r="F28" s="17">
-        <v>1.4999999999999999E-4</v>
-      </c>
-      <c r="G28" t="s">
-        <v>107</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="I28" s="5"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="18" t="s">
-        <v>37</v>
       </c>
       <c r="B29" s="18" t="s">
         <v>60</v>
@@ -2155,23 +2316,29 @@
         <v>8000</v>
       </c>
       <c r="E29" s="17">
-        <f>J29/1000/1000/1000</f>
+        <f>L29/1000/1000/1000</f>
         <v>0</v>
       </c>
       <c r="F29" s="17">
-        <v>4.6999999999999999E-4</v>
-      </c>
-      <c r="G29" t="s">
-        <v>107</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="I29" s="5"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1.4999999999999999E-4</v>
+      </c>
+      <c r="G29" s="17">
+        <v>4</v>
+      </c>
+      <c r="H29" s="17">
+        <f t="shared" si="1"/>
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="I29" s="17">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B30" s="18" t="s">
         <v>60</v>
@@ -2183,26 +2350,32 @@
         <v>8000</v>
       </c>
       <c r="E30" s="17">
-        <f>J30/1000/1000/1000</f>
+        <f>L30/1000/1000/1000</f>
         <v>0</v>
       </c>
       <c r="F30" s="17">
-        <v>1.93E-4</v>
-      </c>
-      <c r="G30" t="s">
-        <v>107</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="I30" s="5"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4.6999999999999999E-4</v>
+      </c>
+      <c r="G30" s="17">
+        <v>2</v>
+      </c>
+      <c r="H30" s="17">
+        <f t="shared" si="1"/>
+        <v>9.3999999999999997E-4</v>
+      </c>
+      <c r="I30" s="17">
+        <f t="shared" si="2"/>
+        <v>0.94</v>
+      </c>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="18" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C31" s="17" t="s">
         <v>49</v>
@@ -2211,234 +2384,223 @@
         <v>8000</v>
       </c>
       <c r="E31" s="17">
-        <f>J31/1000/1000/1000</f>
+        <f>L31/1000/1000/1000</f>
         <v>0</v>
       </c>
       <c r="F31" s="17">
+        <v>1.93E-4</v>
+      </c>
+      <c r="G31" s="17">
+        <v>16</v>
+      </c>
+      <c r="H31" s="17">
+        <f t="shared" si="1"/>
+        <v>3.088E-3</v>
+      </c>
+      <c r="I31" s="17">
+        <f t="shared" si="2"/>
+        <v>3.0880000000000001</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="K31" s="5"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" s="17">
+        <v>8000</v>
+      </c>
+      <c r="E32" s="17">
+        <f>L32/1000/1000/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F32" s="17">
         <f>0.0017</f>
         <v>1.6999999999999999E-3</v>
       </c>
-      <c r="G31" t="s">
-        <v>107</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="I31" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="16" t="s">
+      <c r="G32" s="17">
+        <v>4</v>
+      </c>
+      <c r="H32" s="17">
+        <f t="shared" si="1"/>
+        <v>6.7999999999999996E-3</v>
+      </c>
+      <c r="I32" s="17">
+        <f t="shared" si="2"/>
+        <v>6.8</v>
+      </c>
+      <c r="J32" s="5"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="16"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="H32" s="5"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="18" t="s">
+      <c r="B33" s="16"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J33" s="5"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B33" s="18" t="s">
+      <c r="B34" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C33" s="17" t="s">
+      <c r="C34" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="17">
+      <c r="D34" s="17">
         <v>8000</v>
       </c>
-      <c r="E33" s="17">
-        <f>J33/1000/1000/1000</f>
-        <v>0</v>
-      </c>
-      <c r="F33" s="17">
+      <c r="E34" s="17">
+        <f>L34/1000/1000/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F34" s="17">
         <v>2.2000000000000001E-4</v>
       </c>
-      <c r="G33" t="s">
-        <v>107</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="18" t="s">
+      <c r="G34" s="17">
+        <v>12</v>
+      </c>
+      <c r="H34" s="17">
+        <f t="shared" si="1"/>
+        <v>2.64E-3</v>
+      </c>
+      <c r="I34" s="17">
+        <f t="shared" si="2"/>
+        <v>2.64</v>
+      </c>
+      <c r="J34" s="5"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B35" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="C35" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="D34" s="17">
+      <c r="D35" s="17">
         <v>2700</v>
       </c>
-      <c r="E34" s="17">
-        <f>J34/1000/1000/1000</f>
-        <v>0</v>
-      </c>
-      <c r="F34" s="17">
+      <c r="E35" s="17">
+        <f>L35/1000/1000/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F35" s="17">
         <v>6.9999999999999994E-5</v>
       </c>
-      <c r="G34" t="s">
-        <v>107</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="I34" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="18" t="s">
+      <c r="G35" s="17">
+        <v>12</v>
+      </c>
+      <c r="H35" s="17">
+        <f t="shared" si="1"/>
+        <v>8.3999999999999993E-4</v>
+      </c>
+      <c r="I35" s="17">
+        <f t="shared" si="2"/>
+        <v>0.84</v>
+      </c>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="18" t="s">
+      <c r="B36" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C35" s="17" t="s">
+      <c r="C36" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D35" s="17">
+      <c r="D36" s="17">
         <v>1150</v>
       </c>
-      <c r="E35" s="17">
-        <f>J35/1000/1000/1000</f>
-        <v>0</v>
-      </c>
-      <c r="F35" s="17">
+      <c r="E36" s="17">
+        <f>L36/1000/1000/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F36" s="17">
         <v>4.3000000000000002E-5</v>
       </c>
-      <c r="G35" t="s">
-        <v>107</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="I35" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
-      <c r="F36">
-        <f>SUM(F2:F35)*1000</f>
-        <v>186.696</v>
-      </c>
-      <c r="H36" s="20"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="B38" s="13"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14">
-        <f>J38/1000/1000/1000</f>
-        <v>0</v>
-      </c>
-      <c r="F38" s="14"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="B39" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="D39" s="14">
-        <v>8800</v>
-      </c>
-      <c r="E39" s="14">
-        <v>0.35</v>
-      </c>
-      <c r="F39" s="14"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B40" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="C40" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D40" s="14">
-        <v>1070</v>
-      </c>
-      <c r="E40" s="14">
-        <v>0.4</v>
-      </c>
-      <c r="F40" s="14"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>100</v>
-      </c>
-      <c r="E41" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>154</v>
-      </c>
-      <c r="B44" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>156</v>
-      </c>
-      <c r="B45" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>158</v>
-      </c>
-      <c r="B46" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>159</v>
-      </c>
-      <c r="B47" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>165</v>
-      </c>
-      <c r="B48" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>164</v>
-      </c>
-      <c r="B49">
-        <v>9.5</v>
-      </c>
+      <c r="G36" s="17">
+        <v>0</v>
+      </c>
+      <c r="H36" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I36" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" s="18"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="J38" s="20"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39" s="26"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="27">
+        <f>SUM(H2:H37)-H31</f>
+        <v>0.23277</v>
+      </c>
+      <c r="I39" s="27">
+        <f t="shared" si="2"/>
+        <v>232.77</v>
+      </c>
+      <c r="J39" s="20"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H40" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2446,11 +2608,1248 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A729A410-6F9D-4B69-8564-D96FAE86FB77}">
+  <dimension ref="A1:K55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.77734375" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="29" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1850</v>
+      </c>
+      <c r="E3" s="6">
+        <f t="shared" ref="E3:E16" si="0">L3/1000/1000/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="6">
+        <v>8.3999999999999995E-3</v>
+      </c>
+      <c r="G3" s="6">
+        <v>1</v>
+      </c>
+      <c r="H3" s="6">
+        <f>F3*G3</f>
+        <v>8.3999999999999995E-3</v>
+      </c>
+      <c r="I3" s="6">
+        <f>H3*1000</f>
+        <v>8.4</v>
+      </c>
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1850</v>
+      </c>
+      <c r="E4" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1.66E-2</v>
+      </c>
+      <c r="G4" s="6">
+        <v>1</v>
+      </c>
+      <c r="H4" s="6">
+        <f t="shared" ref="H4:H37" si="1">F4*G4</f>
+        <v>1.66E-2</v>
+      </c>
+      <c r="I4" s="6">
+        <f t="shared" ref="I4:I40" si="2">H4*1000</f>
+        <v>16.600000000000001</v>
+      </c>
+      <c r="J4" s="5"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1850</v>
+      </c>
+      <c r="E5" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F5" s="6">
+        <v>6.6E-3</v>
+      </c>
+      <c r="G5" s="6">
+        <v>1</v>
+      </c>
+      <c r="H5" s="6">
+        <f t="shared" si="1"/>
+        <v>6.6E-3</v>
+      </c>
+      <c r="I5" s="6">
+        <f t="shared" si="2"/>
+        <v>6.6</v>
+      </c>
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="6">
+        <v>1850</v>
+      </c>
+      <c r="E6" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="6">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="G6" s="6">
+        <v>1</v>
+      </c>
+      <c r="H6" s="6">
+        <f t="shared" si="1"/>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="I6" s="6">
+        <f>H6*1000</f>
+        <v>8</v>
+      </c>
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="6">
+        <v>1850</v>
+      </c>
+      <c r="E7" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="6">
+        <v>7.1000000000000004E-3</v>
+      </c>
+      <c r="G7" s="6">
+        <v>1</v>
+      </c>
+      <c r="H7" s="6">
+        <f t="shared" si="1"/>
+        <v>7.1000000000000004E-3</v>
+      </c>
+      <c r="I7" s="6">
+        <f>H7*1000</f>
+        <v>7.1000000000000005</v>
+      </c>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="6">
+        <v>1850</v>
+      </c>
+      <c r="E8" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="6">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="G8" s="6">
+        <v>1</v>
+      </c>
+      <c r="H8" s="6">
+        <f t="shared" si="1"/>
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="I8" s="6">
+        <f>H8*1000</f>
+        <v>7</v>
+      </c>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="6">
+        <v>1850</v>
+      </c>
+      <c r="E9" s="6">
+        <f t="shared" ref="E9" si="3">L9/1000/1000/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="6">
+        <v>1.1299999999999999E-2</v>
+      </c>
+      <c r="G9" s="6">
+        <v>1</v>
+      </c>
+      <c r="H9" s="6">
+        <f t="shared" ref="H9" si="4">F9*G9</f>
+        <v>1.1299999999999999E-2</v>
+      </c>
+      <c r="I9" s="6">
+        <f t="shared" si="2"/>
+        <v>11.299999999999999</v>
+      </c>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="6">
+        <v>1850</v>
+      </c>
+      <c r="E10" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="6">
+        <v>1.11E-2</v>
+      </c>
+      <c r="G10" s="6">
+        <v>3</v>
+      </c>
+      <c r="H10" s="6">
+        <f t="shared" si="1"/>
+        <v>3.3300000000000003E-2</v>
+      </c>
+      <c r="I10" s="6">
+        <f t="shared" si="2"/>
+        <v>33.300000000000004</v>
+      </c>
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="6">
+        <v>5.7000000000000002E-3</v>
+      </c>
+      <c r="G11" s="6">
+        <v>1</v>
+      </c>
+      <c r="H11" s="6">
+        <f t="shared" si="1"/>
+        <v>5.7000000000000002E-3</v>
+      </c>
+      <c r="I11" s="6">
+        <f t="shared" si="2"/>
+        <v>5.7</v>
+      </c>
+      <c r="J11" s="5"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="6">
+        <v>1850</v>
+      </c>
+      <c r="E13" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="6">
+        <v>9.1999999999999998E-3</v>
+      </c>
+      <c r="G13" s="6">
+        <v>1</v>
+      </c>
+      <c r="H13" s="6">
+        <f t="shared" si="1"/>
+        <v>9.1999999999999998E-3</v>
+      </c>
+      <c r="I13" s="6">
+        <f t="shared" si="2"/>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="6">
+        <v>1850</v>
+      </c>
+      <c r="E14" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="6">
+        <v>7.6E-3</v>
+      </c>
+      <c r="G14" s="6">
+        <v>1</v>
+      </c>
+      <c r="H14" s="6">
+        <f t="shared" si="1"/>
+        <v>7.6E-3</v>
+      </c>
+      <c r="I14" s="6">
+        <f t="shared" si="2"/>
+        <v>7.6</v>
+      </c>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="6">
+        <v>2200</v>
+      </c>
+      <c r="E15" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="6">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="G15" s="6">
+        <v>1</v>
+      </c>
+      <c r="H15" s="6">
+        <f t="shared" si="1"/>
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="I15" s="6">
+        <f t="shared" si="2"/>
+        <v>0.7</v>
+      </c>
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="6">
+        <v>2810</v>
+      </c>
+      <c r="E16" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="6">
+        <v>2.4300000000000002E-2</v>
+      </c>
+      <c r="G16" s="6">
+        <v>1</v>
+      </c>
+      <c r="H16" s="6">
+        <f t="shared" si="1"/>
+        <v>2.4300000000000002E-2</v>
+      </c>
+      <c r="I16" s="6">
+        <f t="shared" si="2"/>
+        <v>24.3</v>
+      </c>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="10"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11">
+        <f>L18/1000/1000/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="11">
+        <v>5316</v>
+      </c>
+      <c r="E19" s="11">
+        <f>L19/1000/1000/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="11">
+        <v>9.5E-4</v>
+      </c>
+      <c r="G19" s="11">
+        <v>5</v>
+      </c>
+      <c r="H19" s="11">
+        <f t="shared" si="1"/>
+        <v>4.7499999999999999E-3</v>
+      </c>
+      <c r="I19" s="11">
+        <f t="shared" si="2"/>
+        <v>4.75</v>
+      </c>
+      <c r="J19" s="5"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="11">
+        <v>2750</v>
+      </c>
+      <c r="E20" s="11">
+        <f>L20/1000/1000/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="11">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="G20" s="11">
+        <v>1</v>
+      </c>
+      <c r="H20" s="11">
+        <f t="shared" si="1"/>
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="I20" s="11">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="J20" s="5"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="J21" s="5"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="B22" s="13"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="5"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="14">
+        <v>8800</v>
+      </c>
+      <c r="E23" s="14">
+        <f>L23/1000/1000/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F23" s="28">
+        <v>3.2499999999999999E-4</v>
+      </c>
+      <c r="G23" s="14">
+        <v>14.75</v>
+      </c>
+      <c r="H23" s="14">
+        <f>F23*G23</f>
+        <v>4.7937499999999994E-3</v>
+      </c>
+      <c r="I23" s="14">
+        <f>H23*1000</f>
+        <v>4.7937499999999993</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="14">
+        <v>1070</v>
+      </c>
+      <c r="E24" s="14">
+        <f>L24/1000/1000/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F24" s="28">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="G24" s="14">
+        <v>14.75</v>
+      </c>
+      <c r="H24" s="14">
+        <f>F24*G24</f>
+        <v>5.8999999999999999E-3</v>
+      </c>
+      <c r="I24" s="14">
+        <f>H24*1000</f>
+        <v>5.8999999999999995</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" s="15"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14">
+        <v>7.2499999999999995E-4</v>
+      </c>
+      <c r="G25" s="14">
+        <v>14.75</v>
+      </c>
+      <c r="H25" s="14">
+        <f>F25*G25</f>
+        <v>1.0693749999999998E-2</v>
+      </c>
+      <c r="I25" s="14">
+        <f>H25*1000</f>
+        <v>10.693749999999998</v>
+      </c>
+      <c r="J25" s="5"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="J26" s="5"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="16"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="5"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17">
+        <f>L28/1000/1000/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F28" s="17">
+        <v>0.03</v>
+      </c>
+      <c r="G28" s="17">
+        <v>1</v>
+      </c>
+      <c r="H28" s="17">
+        <f t="shared" si="1"/>
+        <v>0.03</v>
+      </c>
+      <c r="I28" s="17">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="J28" s="5"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="16"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="5"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="17">
+        <v>8000</v>
+      </c>
+      <c r="E30" s="17">
+        <f>L30/1000/1000/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F30" s="17">
+        <v>1.4999999999999999E-4</v>
+      </c>
+      <c r="G30" s="17">
+        <v>4</v>
+      </c>
+      <c r="H30" s="17">
+        <f t="shared" si="1"/>
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="I30" s="17">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" s="17">
+        <v>8000</v>
+      </c>
+      <c r="E31" s="17">
+        <f>L31/1000/1000/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="17">
+        <v>4.6999999999999999E-4</v>
+      </c>
+      <c r="G31" s="17">
+        <v>2</v>
+      </c>
+      <c r="H31" s="17">
+        <f t="shared" si="1"/>
+        <v>9.3999999999999997E-4</v>
+      </c>
+      <c r="I31" s="17">
+        <f t="shared" si="2"/>
+        <v>0.94</v>
+      </c>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" s="17">
+        <v>8000</v>
+      </c>
+      <c r="E32" s="17">
+        <f>L32/1000/1000/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F32" s="17">
+        <v>1.93E-4</v>
+      </c>
+      <c r="G32" s="17">
+        <v>16</v>
+      </c>
+      <c r="H32" s="17">
+        <f t="shared" si="1"/>
+        <v>3.088E-3</v>
+      </c>
+      <c r="I32" s="17">
+        <f t="shared" si="2"/>
+        <v>3.0880000000000001</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="K32" s="5"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" s="17">
+        <v>8000</v>
+      </c>
+      <c r="E33" s="17">
+        <f>L33/1000/1000/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F33" s="17">
+        <f>0.0017</f>
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="G33" s="17">
+        <v>4</v>
+      </c>
+      <c r="H33" s="17">
+        <f t="shared" si="1"/>
+        <v>6.7999999999999996E-3</v>
+      </c>
+      <c r="I33" s="17">
+        <f t="shared" si="2"/>
+        <v>6.8</v>
+      </c>
+      <c r="J33" s="5"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="16"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J34" s="5"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D35" s="17">
+        <v>8000</v>
+      </c>
+      <c r="E35" s="17">
+        <f>L35/1000/1000/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F35" s="17">
+        <v>2.2000000000000001E-4</v>
+      </c>
+      <c r="G35" s="17">
+        <v>12</v>
+      </c>
+      <c r="H35" s="17">
+        <f t="shared" si="1"/>
+        <v>2.64E-3</v>
+      </c>
+      <c r="I35" s="17">
+        <f t="shared" si="2"/>
+        <v>2.64</v>
+      </c>
+      <c r="J35" s="20"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" s="17">
+        <v>2700</v>
+      </c>
+      <c r="E36" s="17">
+        <f>L36/1000/1000/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F36" s="17">
+        <v>6.9999999999999994E-5</v>
+      </c>
+      <c r="G36" s="17">
+        <v>12</v>
+      </c>
+      <c r="H36" s="17">
+        <f t="shared" si="1"/>
+        <v>8.3999999999999993E-4</v>
+      </c>
+      <c r="I36" s="17">
+        <f t="shared" si="2"/>
+        <v>0.84</v>
+      </c>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37" s="17">
+        <v>1150</v>
+      </c>
+      <c r="E37" s="17">
+        <f>L37/1000/1000/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F37" s="17">
+        <v>4.3000000000000002E-5</v>
+      </c>
+      <c r="G37" s="17">
+        <v>0</v>
+      </c>
+      <c r="H37" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I37" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" s="18"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="J39" s="20"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="B40" s="26"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="27">
+        <f>SUM(H2:H38)-H23-H24-H32</f>
+        <v>0.23706374999999996</v>
+      </c>
+      <c r="I40" s="30">
+        <f t="shared" si="2"/>
+        <v>237.06374999999997</v>
+      </c>
+      <c r="J40" s="20"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" s="3"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" s="31"/>
+      <c r="B42" s="31"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="31"/>
+      <c r="F42" s="31"/>
+      <c r="G42" s="31"/>
+      <c r="H42" s="31"/>
+      <c r="I42" s="31"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" s="31"/>
+      <c r="B43" s="31"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="31"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="31"/>
+      <c r="G43" s="31"/>
+      <c r="H43" s="31"/>
+      <c r="I43" s="31"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44" s="32"/>
+      <c r="B44" s="32"/>
+      <c r="C44" s="31"/>
+      <c r="D44" s="31"/>
+      <c r="E44" s="31"/>
+      <c r="F44" s="31"/>
+      <c r="G44" s="31"/>
+      <c r="H44" s="31"/>
+      <c r="I44" s="31"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A45" s="33"/>
+      <c r="B45" s="33"/>
+      <c r="C45" s="31"/>
+      <c r="D45" s="34"/>
+      <c r="E45" s="31"/>
+      <c r="F45" s="31"/>
+      <c r="G45" s="31"/>
+      <c r="H45" s="31"/>
+      <c r="I45" s="31"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" s="33"/>
+      <c r="B46" s="33"/>
+      <c r="C46" s="31"/>
+      <c r="D46" s="31"/>
+      <c r="E46" s="31"/>
+      <c r="F46" s="31"/>
+      <c r="G46" s="31"/>
+      <c r="H46" s="31"/>
+      <c r="I46" s="31"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47" s="31"/>
+      <c r="B47" s="31"/>
+      <c r="C47" s="31"/>
+      <c r="D47" s="31"/>
+      <c r="E47" s="31"/>
+      <c r="F47" s="31"/>
+      <c r="G47" s="31"/>
+      <c r="H47" s="31"/>
+      <c r="I47" s="31"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A48" s="31"/>
+      <c r="B48" s="31"/>
+      <c r="C48" s="31"/>
+      <c r="D48" s="31"/>
+      <c r="E48" s="31"/>
+      <c r="F48" s="31"/>
+      <c r="G48" s="31"/>
+      <c r="H48" s="31"/>
+      <c r="I48" s="31"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="31"/>
+      <c r="B49" s="31"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="31"/>
+      <c r="E49" s="31"/>
+      <c r="F49" s="31"/>
+      <c r="G49" s="31"/>
+      <c r="H49" s="31"/>
+      <c r="I49" s="31"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" s="31"/>
+      <c r="B50" s="31"/>
+      <c r="C50" s="31"/>
+      <c r="D50" s="31"/>
+      <c r="E50" s="31"/>
+      <c r="F50" s="31"/>
+      <c r="G50" s="31"/>
+      <c r="H50" s="31"/>
+      <c r="I50" s="31"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" s="31"/>
+      <c r="B51" s="31"/>
+      <c r="C51" s="31"/>
+      <c r="D51" s="31"/>
+      <c r="E51" s="31"/>
+      <c r="F51" s="31"/>
+      <c r="G51" s="31"/>
+      <c r="H51" s="31"/>
+      <c r="I51" s="31"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" s="31"/>
+      <c r="B52" s="31"/>
+      <c r="C52" s="31"/>
+      <c r="D52" s="31"/>
+      <c r="E52" s="31"/>
+      <c r="F52" s="31"/>
+      <c r="G52" s="31"/>
+      <c r="H52" s="31"/>
+      <c r="I52" s="31"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" s="31"/>
+      <c r="B53" s="31"/>
+      <c r="C53" s="31"/>
+      <c r="D53" s="31"/>
+      <c r="E53" s="31"/>
+      <c r="F53" s="31"/>
+      <c r="G53" s="31"/>
+      <c r="H53" s="31"/>
+      <c r="I53" s="31"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" s="31"/>
+      <c r="B54" s="31"/>
+      <c r="C54" s="31"/>
+      <c r="D54" s="31"/>
+      <c r="E54" s="31"/>
+      <c r="F54" s="31"/>
+      <c r="G54" s="31"/>
+      <c r="H54" s="31"/>
+      <c r="I54" s="31"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" s="31"/>
+      <c r="B55" s="31"/>
+      <c r="C55" s="31"/>
+      <c r="D55" s="31"/>
+      <c r="E55" s="31"/>
+      <c r="F55" s="31"/>
+      <c r="G55" s="31"/>
+      <c r="H55" s="31"/>
+      <c r="I55" s="31"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1282F9C-F5B3-4D06-B4B0-82EDC369CF35}">
   <dimension ref="A1:H106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E102" sqref="E102"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2466,27 +3865,27 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="G2" s="22" t="s">
         <v>4</v>
@@ -2497,7 +3896,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
@@ -2505,32 +3904,32 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="G9" s="22" t="s">
         <v>4</v>
@@ -2541,7 +3940,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -2556,10 +3955,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B11" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D11" t="e">
         <f>C11/C12</f>
@@ -2571,7 +3970,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="23" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B12" t="s">
         <v>23</v>
@@ -2587,22 +3986,22 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="G14" s="22" t="s">
         <v>4</v>
@@ -2613,7 +4012,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
@@ -2628,10 +4027,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B16" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D16" t="e">
         <f>C16/C17</f>
@@ -2643,7 +4042,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="23" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B17" t="s">
         <v>23</v>
@@ -2659,22 +4058,22 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="G19" s="22" t="s">
         <v>4</v>
@@ -2685,7 +4084,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
@@ -2700,10 +4099,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B21" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D21" t="e">
         <f>C21/C22</f>
@@ -2715,7 +4114,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="23" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B22" t="s">
         <v>23</v>
@@ -2731,17 +4130,17 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -2749,22 +4148,22 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="G28" s="22" t="s">
         <v>4</v>
@@ -2775,7 +4174,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="B29" t="s">
         <v>6</v>
@@ -2790,10 +4189,10 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="B30" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D30" t="e">
         <f>C30/C31</f>
@@ -2805,7 +4204,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="23" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B31" t="s">
         <v>23</v>
@@ -2821,22 +4220,22 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="G34" s="22" t="s">
         <v>4</v>
@@ -2847,7 +4246,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B35" t="s">
         <v>6</v>
@@ -2862,10 +4261,10 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="B36" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D36" t="e">
         <f>C36/C37</f>
@@ -2877,7 +4276,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="23" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B37" t="s">
         <v>23</v>
@@ -2893,22 +4292,22 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="G40" s="22" t="s">
         <v>4</v>
@@ -2919,37 +4318,37 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="23" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="G46" s="22" t="s">
         <v>4</v>
@@ -2960,37 +4359,37 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="23" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="G52" s="22" t="s">
         <v>4</v>
@@ -3001,37 +4400,37 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="23" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="G58" s="22" t="s">
         <v>4</v>
@@ -3042,37 +4441,37 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="23" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="G64" s="22" t="s">
         <v>4</v>
@@ -3083,7 +4482,7 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
@@ -3093,12 +4492,12 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="23" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
@@ -3106,22 +4505,22 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="G70" s="22" t="s">
         <v>4</v>
@@ -3132,7 +4531,7 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="23" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
@@ -3145,22 +4544,22 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="G76" s="22" t="s">
         <v>4</v>
@@ -3171,52 +4570,52 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="23" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="G84" s="22" t="s">
         <v>4</v>
@@ -3227,7 +4626,7 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="23" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.3">
@@ -3237,22 +4636,22 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="G89" s="22" t="s">
         <v>4</v>
@@ -3273,17 +4672,17 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="23" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.3">
@@ -3293,22 +4692,22 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="24" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="G98" s="22" t="s">
         <v>4</v>
@@ -3319,7 +4718,7 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" s="25" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B99" t="s">
         <v>52</v>
@@ -3343,12 +4742,12 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="B101" t="s">
         <v>24</v>
@@ -3359,7 +4758,7 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="B102" t="s">
         <v>24</v>
@@ -3371,7 +4770,7 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="B103" t="s">
         <v>24</v>
@@ -3382,7 +4781,7 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="B104" t="s">
         <v>24</v>
@@ -3393,7 +4792,7 @@
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="B105" t="s">
         <v>24</v>
@@ -3404,7 +4803,7 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="B106" t="s">
         <v>24</v>
@@ -3418,7 +4817,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F6B548F-C44E-440B-8115-652E4A726701}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3430,4 +4829,165 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61C9E490-A744-473C-8872-3574F7E7A57E}">
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14">
+        <f>'Masses and Volumes'!L41/1000/1000/1000</f>
+        <v>0</v>
+      </c>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+    </row>
+    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="14">
+        <v>8800</v>
+      </c>
+      <c r="E2" s="14">
+        <v>0.35</v>
+      </c>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="14">
+        <v>1070</v>
+      </c>
+      <c r="E3" s="14">
+        <v>0.4</v>
+      </c>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>153</v>
+      </c>
+      <c r="B11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>152</v>
+      </c>
+      <c r="B12">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>167</v>
+      </c>
+      <c r="B14">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>168</v>
+      </c>
+      <c r="B15">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>169</v>
+      </c>
+      <c r="B16">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>170</v>
+      </c>
+      <c r="B17">
+        <v>11.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Excel Progress + Slider Fix
Old slider board was composed of a single solid, while the real one has a hole on the middle. A 4 piece group has been added to the geometric model and the excel document has been updated  with some PCB Properties and ESATAN volumes.
</commit_message>
<xml_diff>
--- a/PoCat3_Thermal_Model_Mass_Properties.xlsx
+++ b/PoCat3_Thermal_Model_Mass_Properties.xlsx
@@ -9,21 +9,22 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="4"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Materials" sheetId="1" r:id="rId1"/>
     <sheet name="Masses and Volumes" sheetId="8" r:id="rId2"/>
-    <sheet name="Bulks" sheetId="6" r:id="rId3"/>
-    <sheet name="Extra" sheetId="9" r:id="rId4"/>
-    <sheet name="Masses and Volumes Old VC" sheetId="7" r:id="rId5"/>
+    <sheet name="Properties PCBs" sheetId="10" r:id="rId3"/>
+    <sheet name="Bulks" sheetId="6" r:id="rId4"/>
+    <sheet name="Extra" sheetId="9" r:id="rId5"/>
+    <sheet name="Masses and Volumes Old VC" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="227">
   <si>
     <t>Material</t>
   </si>
@@ -610,13 +611,100 @@
     <t>Kband Bot</t>
   </si>
   <si>
-    <t>PP2116</t>
-  </si>
-  <si>
     <t>Cobre</t>
   </si>
   <si>
     <t>Laterales y Bot</t>
+  </si>
+  <si>
+    <t>R= rho* l/A</t>
+  </si>
+  <si>
+    <t>rho= suma[rho_i * w_i]</t>
+  </si>
+  <si>
+    <t>PCB</t>
+  </si>
+  <si>
+    <t>Mask</t>
+  </si>
+  <si>
+    <t>OBC-COMMS</t>
+  </si>
+  <si>
+    <t>Y+Mag</t>
+  </si>
+  <si>
+    <t>Laterals</t>
+  </si>
+  <si>
+    <t>Bottom</t>
+  </si>
+  <si>
+    <t>Copper (mm)</t>
+  </si>
+  <si>
+    <t>FR4  (mm)</t>
+  </si>
+  <si>
+    <t>Mask  (mm)</t>
+  </si>
+  <si>
+    <t>Conductivity (k) [W/m·K] (ip)</t>
+  </si>
+  <si>
+    <t>Conductivity (k) [W/m·K] (cp)</t>
+  </si>
+  <si>
+    <t>FR-4 (ip)</t>
+  </si>
+  <si>
+    <t>FR-4 (cp)</t>
+  </si>
+  <si>
+    <t>(approx)</t>
+  </si>
+  <si>
+    <t>BotLat Bulk</t>
+  </si>
+  <si>
+    <t>Slider Bulk</t>
+  </si>
+  <si>
+    <t>Y+Mag Bulk</t>
+  </si>
+  <si>
+    <t>PCB Bulk</t>
+  </si>
+  <si>
+    <t>Kband(B) Bulk</t>
+  </si>
+  <si>
+    <t>ESATAN Area (m^2)</t>
+  </si>
+  <si>
+    <t>Rogers  (mm)</t>
+  </si>
+  <si>
+    <t>Rogers</t>
+  </si>
+  <si>
+    <t>Kband Top</t>
+  </si>
+  <si>
+    <t>Kband Interface</t>
+  </si>
+  <si>
+    <t>Kband Under</t>
+  </si>
+  <si>
+    <t>Kband Support</t>
+  </si>
+  <si>
+    <t>Kband Antenna</t>
+  </si>
+  <si>
+    <t>Kband Over</t>
   </si>
 </sst>
 </file>
@@ -761,7 +849,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -833,6 +921,14 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -937,6 +1033,121 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1" descr="C:\Users\oscar\OneDrive\Escritorio\resistenciacp.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5124450" y="5057775"/>
+          <a:ext cx="4638675" cy="2476500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2" descr="C:\Users\oscar\OneDrive\Escritorio\resistenciaip.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5114925" y="7705725"/>
+          <a:ext cx="5781675" cy="1685925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1244,7 +1455,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D7" sqref="D7:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1622,7 +1833,7 @@
   <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2715,10 +2926,562 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M34"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="26" customWidth="1"/>
+    <col min="7" max="7" width="30" customWidth="1"/>
+    <col min="8" max="9" width="8.5703125" customWidth="1"/>
+    <col min="10" max="10" width="18" customWidth="1"/>
+    <col min="11" max="11" width="23.5703125" customWidth="1"/>
+    <col min="12" max="12" width="30.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C2">
+        <v>1.44</v>
+      </c>
+      <c r="D2">
+        <v>0.02</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f>1/((1/(B2*$L$2)+1/(C2*$L$4)+1/(D2*$L$5))*(B2+C2+D2+E2))</f>
+        <v>2.4761056482585533E-3</v>
+      </c>
+      <c r="G2">
+        <f>(B2*$L$2+C2*$L$3+D2*$L$5+E2*$L$6)*(B2+C2+D2+E2)</f>
+        <v>91.472640000000013</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="7">
+        <v>8930</v>
+      </c>
+      <c r="K2" s="7">
+        <v>385</v>
+      </c>
+      <c r="L2" s="7">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C3">
+        <v>1.44</v>
+      </c>
+      <c r="D3">
+        <v>0.02</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F8" si="0">1/((1/(B3*$L$2)+1/(C3*$L$4)+1/(D3*$L$5))*(B3+C3+D3+E3))</f>
+        <v>2.4761056482585533E-3</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G9" si="1">(B3*$L$2+C3*$L$3+D3*$L$5+E3*$L$6)*(B3+C3+D3+E3)</f>
+        <v>91.472640000000013</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="J3" s="7">
+        <v>1850</v>
+      </c>
+      <c r="K3" s="7">
+        <v>1200</v>
+      </c>
+      <c r="L3" s="7">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C4">
+        <v>1.44</v>
+      </c>
+      <c r="D4">
+        <v>0.02</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>2.4761056482585533E-3</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>91.472640000000013</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J4" s="7">
+        <v>1850</v>
+      </c>
+      <c r="K4" s="7">
+        <v>1200</v>
+      </c>
+      <c r="L4" s="7">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B5">
+        <v>0.21000000000000002</v>
+      </c>
+      <c r="C5">
+        <v>1.77</v>
+      </c>
+      <c r="D5">
+        <v>0.02</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>1.9844413195134712E-3</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>170.87540000000004</v>
+      </c>
+      <c r="I5" s="35" t="s">
+        <v>200</v>
+      </c>
+      <c r="J5" s="36">
+        <v>2000</v>
+      </c>
+      <c r="K5" s="36">
+        <v>1000</v>
+      </c>
+      <c r="L5" s="36">
+        <v>0.2</v>
+      </c>
+      <c r="M5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>203</v>
+      </c>
+      <c r="B6">
+        <v>0.21000000000000002</v>
+      </c>
+      <c r="C6">
+        <v>1.77</v>
+      </c>
+      <c r="D6">
+        <v>0.02</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>1.9844413195134712E-3</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>170.87540000000004</v>
+      </c>
+      <c r="I6" s="35" t="s">
+        <v>220</v>
+      </c>
+      <c r="J6" s="7">
+        <v>2200</v>
+      </c>
+      <c r="K6" s="7">
+        <v>960</v>
+      </c>
+      <c r="L6" s="7">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>204</v>
+      </c>
+      <c r="B7">
+        <v>0.21000000000000002</v>
+      </c>
+      <c r="C7">
+        <v>1.77</v>
+      </c>
+      <c r="D7">
+        <v>0.02</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>1.9844413195134712E-3</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>170.87540000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C8">
+        <v>1.51</v>
+      </c>
+      <c r="D8">
+        <v>0.02</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>2.4770197889097197E-3</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>46.763360000000006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>223</v>
+      </c>
+      <c r="B9">
+        <v>0.21000000000000002</v>
+      </c>
+      <c r="C9">
+        <v>0.84000000000000008</v>
+      </c>
+      <c r="D9">
+        <v>0.04</v>
+      </c>
+      <c r="E9">
+        <v>0.21</v>
+      </c>
+      <c r="F9">
+        <f>1/((1/(B9*$L$2)+1/(C9*$L$4)+1/(D9*$L$5)+1/(E9*$L$6))*(B9+C9+D9+E9))</f>
+        <v>5.0300678708131551E-3</v>
+      </c>
+      <c r="G9">
+        <f>(B9*$L$2+C9*$L$3+D9*$L$5+E9*$L$6)*(B9+C9+D9+E9)</f>
+        <v>110.14952000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>226</v>
+      </c>
+      <c r="F10" t="e">
+        <f>1/((1/(B10*$L$2)+1/(C10*$L$4)+1/(D10*$L$5)+1/(E10*$L$6))*(B10+C10+D10+E10))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G10">
+        <f>(B10*$L$2+C10*$L$3+D10*$L$5+E10*$L$6)*(B10+C10+D10+E10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="F14" s="37" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>201</v>
+      </c>
+      <c r="B15">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C15">
+        <v>1.44</v>
+      </c>
+      <c r="D15">
+        <v>0.02</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <f>(B15*$J$2*$K$2+C15*$J$3*$K$3+D15*$J$5*$K$5+E15*$J$6*$K$6)/(B15*$J$2+C15*$J$3+D15*$J$5+E15*$J$6)</f>
+        <v>940.29816397754291</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C16">
+        <v>1.44</v>
+      </c>
+      <c r="D16">
+        <v>0.02</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <f t="shared" ref="F16:F22" si="2">(B16*$J$2*$K$2+C16*$J$3*$K$3+D16*$J$5*$K$5+E16*$J$6*$K$6)/(B16*$J$2+C16*$J$3+D16*$J$5+E16*$J$6)</f>
+        <v>940.29816397754291</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C17">
+        <v>1.44</v>
+      </c>
+      <c r="D17">
+        <v>0.02</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="2"/>
+        <v>940.29816397754291</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>202</v>
+      </c>
+      <c r="B18">
+        <v>0.21000000000000002</v>
+      </c>
+      <c r="C18">
+        <v>1.77</v>
+      </c>
+      <c r="D18">
+        <v>0.02</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="2"/>
+        <v>903.96364021734939</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>203</v>
+      </c>
+      <c r="B19">
+        <v>0.21000000000000002</v>
+      </c>
+      <c r="C19">
+        <v>1.77</v>
+      </c>
+      <c r="D19">
+        <v>0.02</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="2"/>
+        <v>903.96364021734939</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>204</v>
+      </c>
+      <c r="B20">
+        <v>0.21000000000000002</v>
+      </c>
+      <c r="C20">
+        <v>1.77</v>
+      </c>
+      <c r="D20">
+        <v>0.02</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="2"/>
+        <v>903.96364021734939</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C21">
+        <v>1.51</v>
+      </c>
+      <c r="D21">
+        <v>0.02</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="2"/>
+        <v>1050.3855606314694</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>223</v>
+      </c>
+      <c r="B22">
+        <v>0.21000000000000002</v>
+      </c>
+      <c r="C22">
+        <v>0.84000000000000008</v>
+      </c>
+      <c r="D22">
+        <v>0.04</v>
+      </c>
+      <c r="E22">
+        <v>0.21</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="2"/>
+        <v>783.19706393372451</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>226</v>
+      </c>
+      <c r="F23" t="e">
+        <f t="shared" ref="F23" si="3">(B23*$J$2*$K$2+C23*$J$3*$K$3+D23*$J$5*$K$5+E23*$J$6*$K$6)/(B23*$J$2+C23*$J$3+D23*$J$5+E23*$J$6)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G24" s="3"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="22"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G31" s="3"/>
+    </row>
+    <row r="34" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G34" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J127"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="F126" sqref="F126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2783,6 +3546,9 @@
       <c r="E3">
         <v>1</v>
       </c>
+      <c r="F3" s="38" t="s">
+        <v>24</v>
+      </c>
       <c r="G3" s="7">
         <v>1070</v>
       </c>
@@ -2797,6 +3563,9 @@
       <c r="A4" s="3" t="s">
         <v>100</v>
       </c>
+      <c r="F4">
+        <v>4.5600000000000001E-7</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -2837,7 +3606,7 @@
         <v>91</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>213</v>
       </c>
       <c r="C10">
         <v>14.2</v>
@@ -2850,16 +3619,16 @@
         <f>C10/C12</f>
         <v>1</v>
       </c>
-      <c r="F10" t="s">
-        <v>23</v>
+      <c r="F10" s="38" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>92</v>
       </c>
-      <c r="F11" t="s">
-        <v>23</v>
+      <c r="F11" s="38" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2881,6 +3650,9 @@
         <f>SUM(E10:E11)</f>
         <v>1</v>
       </c>
+      <c r="F12">
+        <v>6.6560000000000003E-6</v>
+      </c>
       <c r="H12">
         <f>H10*E10+H11*E11</f>
         <v>0</v>
@@ -2924,7 +3696,7 @@
         <v>97</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>214</v>
       </c>
       <c r="C15">
         <v>8.4</v>
@@ -2937,8 +3709,8 @@
         <f>C15/C17</f>
         <v>1</v>
       </c>
-      <c r="F15" t="s">
-        <v>23</v>
+      <c r="F15" s="34" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -2959,7 +3731,7 @@
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -3025,7 +3797,7 @@
         <v>103</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>213</v>
       </c>
       <c r="C20">
         <v>9.8000000000000007</v>
@@ -3039,7 +3811,7 @@
         <v>0.96078431372549011</v>
       </c>
       <c r="F20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -3061,7 +3833,7 @@
         <v>3.9215686274509803E-2</v>
       </c>
       <c r="F21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -3083,6 +3855,9 @@
         <f>SUM(E20:E21)</f>
         <v>0.99999999999999989</v>
       </c>
+      <c r="F22">
+        <v>4.6079999999999998E-6</v>
+      </c>
       <c r="H22">
         <f>H20*E20+H21*E21</f>
         <v>0</v>
@@ -3145,7 +3920,7 @@
         <v>107</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
+        <v>213</v>
       </c>
       <c r="C29">
         <v>9.8000000000000007</v>
@@ -3159,7 +3934,7 @@
         <v>0.94230769230769229</v>
       </c>
       <c r="F29" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -3181,7 +3956,7 @@
         <v>5.7692307692307689E-2</v>
       </c>
       <c r="F30" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -3203,6 +3978,9 @@
         <f>SUM(E29:E30)</f>
         <v>1</v>
       </c>
+      <c r="F31">
+        <v>4.6079999999999998E-6</v>
+      </c>
       <c r="H31">
         <f>H29*E29+H30*E30</f>
         <v>0</v>
@@ -3247,7 +4025,7 @@
         <v>108</v>
       </c>
       <c r="B35" t="s">
-        <v>6</v>
+        <v>215</v>
       </c>
       <c r="C35">
         <v>6.6</v>
@@ -3261,7 +4039,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F35" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -3276,7 +4054,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="F36" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -3286,6 +4064,9 @@
       <c r="B37" t="s">
         <v>23</v>
       </c>
+      <c r="F37">
+        <v>4.0500000000000002E-6</v>
+      </c>
       <c r="H37" t="e">
         <f>H35*E35+H36*E36</f>
         <v>#DIV/0!</v>
@@ -3328,6 +4109,9 @@
       <c r="A41" t="s">
         <v>112</v>
       </c>
+      <c r="B41" t="s">
+        <v>216</v>
+      </c>
       <c r="C41">
         <v>5.6</v>
       </c>
@@ -3335,6 +4119,9 @@
         <f>C41/1000</f>
         <v>5.5999999999999999E-3</v>
       </c>
+      <c r="F41" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -3343,11 +4130,17 @@
       <c r="C42">
         <v>2.4</v>
       </c>
+      <c r="F42" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="23" t="s">
         <v>93</v>
       </c>
+      <c r="F43">
+        <v>2.5600000000000001E-6</v>
+      </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
@@ -3382,6 +4175,9 @@
       <c r="A47" t="s">
         <v>113</v>
       </c>
+      <c r="B47" t="s">
+        <v>216</v>
+      </c>
       <c r="C47">
         <v>5.5</v>
       </c>
@@ -3389,6 +4185,9 @@
         <f>C47/1000</f>
         <v>5.4999999999999997E-3</v>
       </c>
+      <c r="F47" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
@@ -3397,11 +4196,17 @@
       <c r="C48">
         <v>1.6</v>
       </c>
+      <c r="F48" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="23" t="s">
         <v>93</v>
       </c>
+      <c r="F49">
+        <v>2.5600000000000001E-6</v>
+      </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
@@ -3436,6 +4241,9 @@
       <c r="A53" t="s">
         <v>114</v>
       </c>
+      <c r="B53" t="s">
+        <v>216</v>
+      </c>
       <c r="C53">
         <v>5.4</v>
       </c>
@@ -3443,6 +4251,9 @@
         <f>C53/1000</f>
         <v>5.4000000000000003E-3</v>
       </c>
+      <c r="F53" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
@@ -3451,11 +4262,17 @@
       <c r="C54">
         <v>1.6</v>
       </c>
+      <c r="F54" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="23" t="s">
         <v>93</v>
       </c>
+      <c r="F55">
+        <v>2.5600000000000001E-6</v>
+      </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
@@ -3490,6 +4307,9 @@
       <c r="A59" t="s">
         <v>183</v>
       </c>
+      <c r="B59" t="s">
+        <v>217</v>
+      </c>
       <c r="C59">
         <v>9.1999999999999993</v>
       </c>
@@ -3497,11 +4317,17 @@
         <f>C59/1000</f>
         <v>9.1999999999999998E-3</v>
       </c>
+      <c r="F59" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="23" t="s">
         <v>93</v>
       </c>
+      <c r="F60">
+        <v>2.5600000000000001E-6</v>
+      </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
@@ -3539,6 +4365,9 @@
       <c r="C65">
         <v>7.6</v>
       </c>
+      <c r="F65" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
@@ -3547,16 +4376,25 @@
       <c r="C66">
         <v>0.7</v>
       </c>
+      <c r="F66" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>92</v>
       </c>
+      <c r="F67" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="23" t="s">
         <v>93</v>
       </c>
+      <c r="F68">
+        <v>2.5600000000000001E-6</v>
+      </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="23"/>
@@ -3578,7 +4416,7 @@
         <v>95</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>87</v>
+        <v>218</v>
       </c>
       <c r="G70" s="2" t="s">
         <v>5</v>
@@ -3601,6 +4439,9 @@
         <f>C71/1000</f>
         <v>5.7000000000000002E-3</v>
       </c>
+      <c r="F71">
+        <v>4.2999999999999999E-4</v>
+      </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="23"/>
@@ -3638,9 +4479,15 @@
       <c r="A74" s="25" t="s">
         <v>130</v>
       </c>
+      <c r="B74" t="s">
+        <v>53</v>
+      </c>
+      <c r="C74">
+        <v>24.3</v>
+      </c>
       <c r="D74">
         <f>C74/1000</f>
-        <v>0</v>
+        <v>2.4300000000000002E-2</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>24</v>
@@ -3667,6 +4514,9 @@
       <c r="C76" t="s">
         <v>24</v>
       </c>
+      <c r="F76">
+        <v>3.1203999999999998E-6</v>
+      </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
@@ -3678,7 +4528,9 @@
       <c r="C77" t="s">
         <v>24</v>
       </c>
-      <c r="F77" s="3"/>
+      <c r="F77" s="32">
+        <v>1.52E-5</v>
+      </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
@@ -3690,6 +4542,9 @@
       <c r="C78" t="s">
         <v>24</v>
       </c>
+      <c r="F78">
+        <v>3.3600000000000003E-8</v>
+      </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
@@ -3701,6 +4556,9 @@
       <c r="C79" t="s">
         <v>24</v>
       </c>
+      <c r="F79">
+        <v>1.92E-8</v>
+      </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
@@ -3716,6 +4574,10 @@
       <c r="A82" s="23" t="s">
         <v>93</v>
       </c>
+      <c r="F82">
+        <f>F76+F77+F78*4+F79*4</f>
+        <v>1.8531600000000001E-5</v>
+      </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="10" t="s">
@@ -3762,6 +4624,9 @@
         <f>C88/1000</f>
         <v>8.9999999999999998E-4</v>
       </c>
+      <c r="F88">
+        <v>3.96E-7</v>
+      </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
@@ -3828,6 +4693,9 @@
         <f>C96/1000</f>
         <v>3.4000000000000002E-2</v>
       </c>
+      <c r="F96">
+        <v>1.216E-5</v>
+      </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="13" t="s">
@@ -3887,6 +4755,9 @@
       <c r="A103" s="23" t="s">
         <v>93</v>
       </c>
+      <c r="F103">
+        <v>2.8980000000000001E-7</v>
+      </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
@@ -3977,6 +4848,9 @@
       <c r="C112" t="s">
         <v>24</v>
       </c>
+      <c r="F112">
+        <v>2.6599999999999999E-6</v>
+      </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
@@ -3988,7 +4862,9 @@
       <c r="C113" t="s">
         <v>24</v>
       </c>
-      <c r="F113" s="3"/>
+      <c r="F113" s="32">
+        <v>7.9800000000000003E-7</v>
+      </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
@@ -4000,6 +4876,9 @@
       <c r="C114" t="s">
         <v>24</v>
       </c>
+      <c r="F114">
+        <v>7.9800000000000003E-7</v>
+      </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
@@ -4011,6 +4890,9 @@
       <c r="C115" t="s">
         <v>24</v>
       </c>
+      <c r="F115">
+        <v>2.9440000000000001E-6</v>
+      </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
@@ -4022,6 +4904,9 @@
       <c r="C116" t="s">
         <v>24</v>
       </c>
+      <c r="F116">
+        <v>2.9440000000000001E-6</v>
+      </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
@@ -4033,11 +4918,18 @@
       <c r="C117" t="s">
         <v>24</v>
       </c>
+      <c r="F117">
+        <v>5.2440000000000001E-6</v>
+      </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="23" t="s">
         <v>93</v>
       </c>
+      <c r="F118">
+        <f>SUM(F112:F117)</f>
+        <v>1.5387999999999999E-5</v>
+      </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="3"/>
@@ -4080,21 +4972,33 @@
       <c r="A122" t="s">
         <v>178</v>
       </c>
+      <c r="F122" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>179</v>
       </c>
+      <c r="F123" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="33" t="s">
         <v>180</v>
       </c>
+      <c r="F124" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="23" t="s">
         <v>93</v>
       </c>
+      <c r="F125">
+        <v>1.3E-7</v>
+      </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
@@ -4108,15 +5012,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:O84"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="I44" sqref="I43:I44"/>
+    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4259,7 +5164,7 @@
         <v>11.2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>168</v>
       </c>
@@ -4267,7 +5172,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>184</v>
       </c>
@@ -4275,7 +5180,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>185</v>
       </c>
@@ -4288,8 +5193,18 @@
       <c r="D25">
         <v>3.5000000000000003E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <f>D25*B25</f>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G25" t="s">
+        <v>197</v>
+      </c>
+      <c r="I25" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>187</v>
       </c>
@@ -4302,8 +5217,12 @@
       <c r="D26">
         <v>0.48</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <f t="shared" ref="E26:E27" si="0">D26*B26</f>
+        <v>1.44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>188</v>
       </c>
@@ -4316,13 +5235,17 @@
       <c r="D27">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>185</v>
       </c>
@@ -4335,8 +5258,12 @@
       <c r="D31">
         <v>3.5000000000000003E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <f>D31*B31</f>
+        <v>0.21000000000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>187</v>
       </c>
@@ -4349,8 +5276,12 @@
       <c r="D32">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <f t="shared" ref="E32:E33" si="1">D32*B32</f>
+        <v>0.30000000000000004</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>187</v>
       </c>
@@ -4363,8 +5294,12 @@
       <c r="D33">
         <v>0.73499999999999999</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <f t="shared" si="1"/>
+        <v>1.47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>188</v>
       </c>
@@ -4377,13 +5312,17 @@
       <c r="D34">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <f>D34*B34</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>185</v>
       </c>
@@ -4396,8 +5335,12 @@
       <c r="D37">
         <v>3.5000000000000003E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <f>D37*B37</f>
+        <v>0.21000000000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>187</v>
       </c>
@@ -4410,8 +5353,12 @@
       <c r="D38">
         <v>0.35399999999999998</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <f t="shared" ref="E38:E39" si="2">D38*B38</f>
+        <v>1.77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>188</v>
       </c>
@@ -4424,13 +5371,20 @@
       <c r="D39">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <f t="shared" si="2"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="O41" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>195</v>
       </c>
@@ -4441,72 +5395,92 @@
         <v>193</v>
       </c>
       <c r="D42">
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="E42">
+        <f>D42*B42</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="B43">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C43" t="s">
         <v>193</v>
       </c>
       <c r="D43">
-        <v>3.5000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1.51</v>
+      </c>
+      <c r="E43">
+        <f t="shared" ref="E43:E44" si="3">D43*B43</f>
+        <v>1.51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B44">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C44" t="s">
         <v>193</v>
       </c>
       <c r="D44">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.01</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="3"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>65</v>
-      </c>
-      <c r="G46" s="3"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="B47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C47" t="s">
         <v>193</v>
       </c>
       <c r="D47">
-        <v>3.5000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.21</v>
+      </c>
+      <c r="E47">
+        <f>D47*B47</f>
+        <v>0.21</v>
+      </c>
+      <c r="G47" s="3"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="B48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C48" t="s">
         <v>193</v>
       </c>
       <c r="D48">
-        <v>1.51</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="E48">
+        <f t="shared" ref="E48" si="4">D48*B48</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>188</v>
       </c>
@@ -4519,17 +5493,285 @@
       <c r="D49">
         <v>0.01</v>
       </c>
+      <c r="E49">
+        <f>D49*B49</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>187</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52" t="s">
+        <v>193</v>
+      </c>
+      <c r="D52">
+        <v>0.91</v>
+      </c>
+      <c r="E52">
+        <f>D52*B52</f>
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>195</v>
+      </c>
+      <c r="B53">
+        <v>2</v>
+      </c>
+      <c r="C53" t="s">
+        <v>193</v>
+      </c>
+      <c r="D53">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="E53">
+        <f t="shared" ref="E53" si="5">D53*B53</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>188</v>
+      </c>
+      <c r="B54">
+        <v>2</v>
+      </c>
+      <c r="C54" t="s">
+        <v>193</v>
+      </c>
+      <c r="D54">
+        <v>0.01</v>
+      </c>
+      <c r="E54">
+        <f>D54*B54</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>220</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70" t="s">
+        <v>193</v>
+      </c>
+      <c r="D70">
+        <v>0.21</v>
+      </c>
+      <c r="E70">
+        <f>D70*B70</f>
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>195</v>
+      </c>
+      <c r="B71">
+        <v>2</v>
+      </c>
+      <c r="C71" t="s">
+        <v>193</v>
+      </c>
+      <c r="D71">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="E71">
+        <f t="shared" ref="E71" si="6">D71*B71</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>188</v>
+      </c>
+      <c r="B72">
+        <v>2</v>
+      </c>
+      <c r="C72" t="s">
+        <v>193</v>
+      </c>
+      <c r="D72">
+        <v>0.01</v>
+      </c>
+      <c r="E72">
+        <f>D72*B72</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>187</v>
+      </c>
+      <c r="B76">
+        <v>3</v>
+      </c>
+      <c r="C76" t="s">
+        <v>193</v>
+      </c>
+      <c r="D76">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E76">
+        <f>D76*B76</f>
+        <v>0.84000000000000008</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>195</v>
+      </c>
+      <c r="B77">
+        <v>4</v>
+      </c>
+      <c r="C77" t="s">
+        <v>193</v>
+      </c>
+      <c r="D77">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="E77">
+        <f t="shared" ref="E77" si="7">D77*B77</f>
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>188</v>
+      </c>
+      <c r="B78">
+        <v>2</v>
+      </c>
+      <c r="C78" t="s">
+        <v>193</v>
+      </c>
+      <c r="D78">
+        <v>0.01</v>
+      </c>
+      <c r="E78">
+        <f>D78*B78</f>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>187</v>
+      </c>
+      <c r="B81">
+        <f>E76</f>
+        <v>0.84000000000000008</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>220</v>
+      </c>
+      <c r="B82">
+        <f>E70</f>
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>195</v>
+      </c>
+      <c r="B83">
+        <f>E71+E77</f>
+        <v>0.21000000000000002</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>188</v>
+      </c>
+      <c r="B84">
+        <f>E72+E78</f>
+        <v>0.04</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
NGTM, Rename PCBs, Bulk Update
Updated and assigned some bulks, placed the NGTM of AOCS,EPS,OBC. Missing PL Under and Over, to discuss with expert perhaps. Renamed stack PCBs. Created some geometry groups.
</commit_message>
<xml_diff>
--- a/PoCat3_Thermal_Model_Mass_Properties.xlsx
+++ b/PoCat3_Thermal_Model_Mass_Properties.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oscar\Documents\GitHub\PoCat-Thermal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oscar\OneDrive\Documentos\GitHub\PoCat-Thermal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D8F6BB-D67C-420C-818B-91B3B494804F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="22992" windowHeight="12324" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="22995" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Materials" sheetId="1" r:id="rId1"/>
@@ -20,12 +19,12 @@
     <sheet name="Extra" sheetId="9" r:id="rId5"/>
     <sheet name="Masses and Volumes Old VC" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="259">
   <si>
     <t>Material</t>
   </si>
@@ -830,7 +829,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1259,7 +1258,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Bueno" xfId="1" builtinId="26"/>
+    <cellStyle name="Buena" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
@@ -1383,7 +1382,7 @@
         <xdr:cNvPr id="2" name="Imagen 1" descr="C:\Users\oscar\OneDrive\Escritorio\resistenciacp.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1444,7 +1443,7 @@
         <xdr:cNvPr id="3" name="Imagen 2" descr="C:\Users\oscar\OneDrive\Escritorio\resistenciaip.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1491,15 +1490,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A1:F17" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6">
-  <autoFilter ref="A1:F17" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:F17" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8" tableBorderDxfId="6">
+  <autoFilter ref="A1:F17"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Material" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Solar Absorptivity (αs)" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="IR Emissivity (εIR)" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Density (ρ) [kg/m³]" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Specific heat (cp) [J/kg·K]" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Conductivity (k) [W/m·K]" dataDxfId="0"/>
+    <tableColumn id="1" name="Material" dataDxfId="5"/>
+    <tableColumn id="2" name="Solar Absorptivity (αs)" dataDxfId="4"/>
+    <tableColumn id="3" name="IR Emissivity (εIR)" dataDxfId="3"/>
+    <tableColumn id="4" name="Density (ρ) [kg/m³]" dataDxfId="2"/>
+    <tableColumn id="5" name="Specific heat (cp) [J/kg·K]" dataDxfId="1"/>
+    <tableColumn id="6" name="Conductivity (k) [W/m·K]" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1581,23 +1580,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1633,23 +1615,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1825,24 +1790,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.109375" customWidth="1"/>
-    <col min="2" max="2" width="21.5546875" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" customWidth="1"/>
-    <col min="5" max="5" width="26.5546875" customWidth="1"/>
-    <col min="6" max="6" width="23.6640625" customWidth="1"/>
+    <col min="1" max="1" width="36.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1862,7 +1827,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1882,7 +1847,7 @@
         <v>8181</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1902,7 +1867,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -1922,15 +1887,15 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>23</v>
+      <c r="C5" s="7">
+        <v>0.7</v>
       </c>
       <c r="D5" s="7">
         <v>8000</v>
@@ -1942,15 +1907,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="7">
-        <v>0</v>
+        <v>0.18</v>
       </c>
       <c r="C6" s="7">
-        <v>0</v>
+        <v>0.21</v>
       </c>
       <c r="D6" s="7">
         <v>2810</v>
@@ -1962,7 +1927,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -1982,7 +1947,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -2002,7 +1967,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -2022,7 +1987,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -2042,7 +2007,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -2062,7 +2027,7 @@
         <v>0.29599999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -2082,7 +2047,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -2102,7 +2067,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -2122,7 +2087,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
@@ -2142,7 +2107,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>20</v>
       </c>
@@ -2162,7 +2127,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -2182,26 +2147,26 @@
         <v>0.16200000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>256</v>
       </c>
       <c r="B20">
-        <v>0.27</v>
+        <v>0.19</v>
       </c>
       <c r="C20">
-        <v>0.86</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>257</v>
       </c>
@@ -2209,16 +2174,16 @@
         <v>0.96</v>
       </c>
       <c r="C21">
-        <v>0.87</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E24" s="3"/>
     </row>
   </sheetData>
@@ -2230,29 +2195,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.109375" customWidth="1"/>
-    <col min="9" max="9" width="13.109375" customWidth="1"/>
-    <col min="10" max="10" width="27.5546875" customWidth="1"/>
-    <col min="11" max="11" width="20.33203125" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" customWidth="1"/>
+    <col min="10" max="10" width="27.5703125" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -2284,7 +2249,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>88</v>
       </c>
@@ -2300,7 +2265,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>43</v>
       </c>
@@ -2333,7 +2298,7 @@
       </c>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>74</v>
       </c>
@@ -2366,7 +2331,7 @@
       </c>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>155</v>
       </c>
@@ -2399,7 +2364,7 @@
       </c>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>156</v>
       </c>
@@ -2432,7 +2397,7 @@
       </c>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>157</v>
       </c>
@@ -2465,7 +2430,7 @@
       </c>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>158</v>
       </c>
@@ -2498,7 +2463,7 @@
       </c>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>167</v>
       </c>
@@ -2531,7 +2496,7 @@
       </c>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>75</v>
       </c>
@@ -2564,7 +2529,7 @@
       </c>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>84</v>
       </c>
@@ -2595,7 +2560,7 @@
       </c>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>29</v>
       </c>
@@ -2609,7 +2574,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>80</v>
       </c>
@@ -2642,7 +2607,7 @@
       </c>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>79</v>
       </c>
@@ -2675,7 +2640,7 @@
       </c>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>45</v>
       </c>
@@ -2708,7 +2673,7 @@
       </c>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>46</v>
       </c>
@@ -2741,12 +2706,12 @@
       </c>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>41</v>
       </c>
@@ -2763,7 +2728,7 @@
       <c r="I18" s="11"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>42</v>
       </c>
@@ -2796,7 +2761,7 @@
       </c>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>16</v>
       </c>
@@ -2829,12 +2794,12 @@
       </c>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="J21" s="5"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>136</v>
       </c>
@@ -2848,7 +2813,7 @@
       <c r="I22" s="14"/>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>160</v>
       </c>
@@ -2883,7 +2848,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>55</v>
       </c>
@@ -2918,7 +2883,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
         <v>92</v>
       </c>
@@ -2942,12 +2907,12 @@
       </c>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>28</v>
       </c>
@@ -2961,7 +2926,7 @@
       <c r="I27" s="17"/>
       <c r="J27" s="5"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
         <v>44</v>
       </c>
@@ -2992,7 +2957,7 @@
       </c>
       <c r="J28" s="5"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
         <v>47</v>
       </c>
@@ -3006,7 +2971,7 @@
       <c r="I29" s="19"/>
       <c r="J29" s="5"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
         <v>35</v>
       </c>
@@ -3040,7 +3005,7 @@
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
         <v>36</v>
       </c>
@@ -3074,7 +3039,7 @@
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
         <v>37</v>
       </c>
@@ -3110,7 +3075,7 @@
       </c>
       <c r="K32" s="5"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
         <v>57</v>
       </c>
@@ -3144,7 +3109,7 @@
       </c>
       <c r="J33" s="5"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
         <v>27</v>
       </c>
@@ -3161,7 +3126,7 @@
       </c>
       <c r="J34" s="5"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
         <v>38</v>
       </c>
@@ -3194,7 +3159,7 @@
       </c>
       <c r="J35" s="20"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
         <v>39</v>
       </c>
@@ -3228,7 +3193,7 @@
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
         <v>40</v>
       </c>
@@ -3262,7 +3227,7 @@
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="18"/>
       <c r="B38" s="18"/>
       <c r="C38" s="17"/>
@@ -3278,12 +3243,12 @@
       <c r="J38" s="5"/>
       <c r="K38" s="5"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="J39" s="20"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="24" t="s">
         <v>92</v>
       </c>
@@ -3303,19 +3268,19 @@
       </c>
       <c r="J40" s="20"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="29"/>
       <c r="B44" s="29"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
     </row>
@@ -3326,30 +3291,30 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView zoomScale="88" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="23.109375" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
     <col min="6" max="6" width="36" customWidth="1"/>
-    <col min="7" max="7" width="39.109375" customWidth="1"/>
-    <col min="8" max="8" width="35.88671875" customWidth="1"/>
-    <col min="9" max="9" width="8.5546875" customWidth="1"/>
+    <col min="7" max="7" width="39.140625" customWidth="1"/>
+    <col min="8" max="8" width="35.85546875" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" customWidth="1"/>
     <col min="10" max="10" width="18" customWidth="1"/>
-    <col min="11" max="11" width="23.5546875" customWidth="1"/>
-    <col min="12" max="12" width="30.88671875" customWidth="1"/>
+    <col min="11" max="11" width="23.5703125" customWidth="1"/>
+    <col min="12" max="12" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -3378,7 +3343,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -3411,7 +3376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>208</v>
       </c>
@@ -3444,7 +3409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>209</v>
       </c>
@@ -3477,7 +3442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>198</v>
       </c>
@@ -3513,7 +3478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>217</v>
       </c>
@@ -3546,7 +3511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
         <v>202</v>
       </c>
@@ -3567,7 +3532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
         <v>64</v>
       </c>
@@ -3588,7 +3553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F9" t="s">
         <v>220</v>
       </c>
@@ -3609,7 +3574,7 @@
         <v>0.11633470148314154</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
         <v>223</v>
       </c>
@@ -3630,8 +3595,8 @@
         <v>0.14107548598838676</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="64" t="s">
         <v>197</v>
       </c>
@@ -3657,7 +3622,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>199</v>
       </c>
@@ -3686,7 +3651,7 @@
         <v>91.472640000000013</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -3715,7 +3680,7 @@
         <v>91.472640000000013</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>66</v>
       </c>
@@ -3744,7 +3709,7 @@
         <v>91.472640000000013</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>200</v>
       </c>
@@ -3773,7 +3738,7 @@
         <v>170.87540000000004</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>201</v>
       </c>
@@ -3802,7 +3767,7 @@
         <v>170.87540000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>202</v>
       </c>
@@ -3831,7 +3796,7 @@
         <v>170.87540000000004</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>64</v>
       </c>
@@ -3860,7 +3825,7 @@
         <v>46.763360000000006</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>220</v>
       </c>
@@ -3889,7 +3854,7 @@
         <v>110.14952000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>223</v>
       </c>
@@ -3918,7 +3883,7 @@
         <v>88.525164000000032</v>
       </c>
     </row>
-    <row r="34" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G34" s="3"/>
     </row>
   </sheetData>
@@ -3928,28 +3893,28 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L139"/>
   <sheetViews>
     <sheetView topLeftCell="C52" zoomScale="68" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G88" sqref="G88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" customWidth="1"/>
-    <col min="3" max="4" width="17.6640625" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.88671875" customWidth="1"/>
-    <col min="7" max="7" width="18.5546875" customWidth="1"/>
-    <col min="8" max="8" width="23.6640625" customWidth="1"/>
-    <col min="9" max="9" width="27.44140625" customWidth="1"/>
-    <col min="10" max="10" width="27.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.44140625" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" customWidth="1"/>
+    <col min="8" max="8" width="23.7109375" customWidth="1"/>
+    <col min="9" max="9" width="27.42578125" customWidth="1"/>
+    <col min="10" max="10" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>88</v>
       </c>
@@ -3957,7 +3922,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
         <v>97</v>
       </c>
@@ -3987,7 +3952,7 @@
       </c>
       <c r="J2" s="22"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="43" t="s">
         <v>92</v>
       </c>
@@ -4018,7 +3983,7 @@
         <v>0.16200000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="68" t="s">
         <v>98</v>
       </c>
@@ -4031,7 +3996,7 @@
       <c r="H4" s="17"/>
       <c r="I4" s="69"/>
     </row>
-    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
         <v>99</v>
       </c>
@@ -4052,8 +4017,8 @@
         <v>0.16200000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="51" t="s">
         <v>89</v>
       </c>
@@ -4085,7 +4050,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="42" t="s">
         <v>90</v>
       </c>
@@ -4120,7 +4085,7 @@
         <v>170.87540000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="42" t="s">
         <v>91</v>
       </c>
@@ -4152,7 +4117,7 @@
         <v>170.87540000000004</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="37" t="s">
         <v>92</v>
       </c>
@@ -4189,8 +4154,8 @@
         <v>170.87540000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
         <v>225</v>
       </c>
@@ -4222,7 +4187,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="34" t="s">
         <v>224</v>
       </c>
@@ -4255,13 +4220,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="36" t="s">
         <v>95</v>
       </c>
       <c r="J17" s="35"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="53" t="s">
         <v>226</v>
       </c>
@@ -4294,7 +4259,7 @@
         <v>46.763360000000006</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="53" t="s">
         <v>227</v>
       </c>
@@ -4327,7 +4292,7 @@
         <v>46.763360000000006</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="53" t="s">
         <v>228</v>
       </c>
@@ -4360,7 +4325,7 @@
         <v>46.763360000000006</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="53" t="s">
         <v>229</v>
       </c>
@@ -4393,7 +4358,7 @@
         <v>46.763360000000006</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="37" t="s">
         <v>92</v>
       </c>
@@ -4429,11 +4394,11 @@
         <v>46.763360000000006</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="23"/>
     </row>
-    <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="51" t="s">
         <v>100</v>
       </c>
@@ -4466,7 +4431,7 @@
       </c>
       <c r="L25" s="22"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="42" t="s">
         <v>101</v>
       </c>
@@ -4500,7 +4465,7 @@
         <v>170.87540000000004</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="42" t="s">
         <v>91</v>
       </c>
@@ -4534,7 +4499,7 @@
         <v>170.87540000000004</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="43" t="s">
         <v>92</v>
       </c>
@@ -4570,7 +4535,7 @@
         <v>170.87540000000004</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="68" t="s">
         <v>98</v>
       </c>
@@ -4584,7 +4549,7 @@
       <c r="I29" s="17"/>
       <c r="J29" s="69"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="52" t="s">
         <v>122</v>
       </c>
@@ -4614,7 +4579,7 @@
         <v>170.87540000000004</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="54" t="s">
         <v>121</v>
       </c>
@@ -4644,11 +4609,11 @@
         <v>170.87540000000004</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
     </row>
-    <row r="33" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="51" t="s">
         <v>102</v>
       </c>
@@ -4681,7 +4646,7 @@
       </c>
       <c r="L34" s="22"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="42" t="s">
         <v>105</v>
       </c>
@@ -4715,7 +4680,7 @@
         <v>170.87540000000004</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="42" t="s">
         <v>103</v>
       </c>
@@ -4749,7 +4714,7 @@
         <v>170.87540000000004</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="37" t="s">
         <v>92</v>
       </c>
@@ -4785,8 +4750,8 @@
         <v>170.87540000000004</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="51" t="s">
         <v>104</v>
       </c>
@@ -4819,7 +4784,7 @@
       </c>
       <c r="L40" s="22"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="42" t="s">
         <v>106</v>
       </c>
@@ -4853,7 +4818,7 @@
         <v>170.87540000000004</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="42" t="s">
         <v>91</v>
       </c>
@@ -4887,7 +4852,7 @@
         <v>170.87540000000004</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="37" t="s">
         <v>92</v>
       </c>
@@ -4919,8 +4884,8 @@
         <v>170.87540000000004</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="51" t="s">
         <v>107</v>
       </c>
@@ -4952,7 +4917,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="42" t="s">
         <v>110</v>
       </c>
@@ -4986,7 +4951,7 @@
         <v>91.472640000000013</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="42" t="s">
         <v>91</v>
       </c>
@@ -5017,7 +4982,7 @@
         <v>91.472640000000013</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="37" t="s">
         <v>92</v>
       </c>
@@ -5051,8 +5016,8 @@
         <v>91.472640000000013</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="51" t="s">
         <v>108</v>
       </c>
@@ -5084,7 +5049,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="42" t="s">
         <v>111</v>
       </c>
@@ -5118,7 +5083,7 @@
         <v>91.472640000000013</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="42" t="s">
         <v>91</v>
       </c>
@@ -5149,7 +5114,7 @@
         <v>91.472640000000013</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="37" t="s">
         <v>92</v>
       </c>
@@ -5183,8 +5148,8 @@
         <v>91.472640000000013</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="51" t="s">
         <v>109</v>
       </c>
@@ -5216,7 +5181,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="42" t="s">
         <v>112</v>
       </c>
@@ -5250,7 +5215,7 @@
         <v>91.472640000000013</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="42" t="s">
         <v>91</v>
       </c>
@@ -5281,7 +5246,7 @@
         <v>91.472640000000013</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="37" t="s">
         <v>92</v>
       </c>
@@ -5315,8 +5280,8 @@
         <v>91.472640000000013</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="51" t="s">
         <v>113</v>
       </c>
@@ -5348,7 +5313,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="42" t="s">
         <v>181</v>
       </c>
@@ -5381,7 +5346,7 @@
         <v>110.14952000000002</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="37" t="s">
         <v>92</v>
       </c>
@@ -5412,8 +5377,8 @@
         <v>110.14952000000002</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="51" t="s">
         <v>114</v>
       </c>
@@ -5446,7 +5411,7 @@
       </c>
       <c r="L69" s="22"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="42" t="s">
         <v>115</v>
       </c>
@@ -5465,7 +5430,7 @@
       </c>
       <c r="J70" s="35"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="42" t="s">
         <v>69</v>
       </c>
@@ -5484,7 +5449,7 @@
       </c>
       <c r="J71" s="35"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="42" t="s">
         <v>91</v>
       </c>
@@ -5497,7 +5462,7 @@
       </c>
       <c r="J72" s="35"/>
     </row>
-    <row r="73" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="37" t="s">
         <v>92</v>
       </c>
@@ -5528,10 +5493,10 @@
         <v>88.525164000000032</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="23"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="41" t="s">
         <v>126</v>
       </c>
@@ -5563,7 +5528,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="37" t="s">
         <v>92</v>
       </c>
@@ -5593,10 +5558,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="23"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="30" t="s">
         <v>168</v>
       </c>
@@ -5628,7 +5593,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="34" t="s">
         <v>128</v>
       </c>
@@ -5663,7 +5628,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="34" t="s">
         <v>250</v>
       </c>
@@ -5695,13 +5660,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="36" t="s">
         <v>169</v>
       </c>
       <c r="J81" s="35"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="53" t="s">
         <v>170</v>
       </c>
@@ -5727,7 +5692,7 @@
         <v>121.26828892653627</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="53" t="s">
         <v>171</v>
       </c>
@@ -5753,7 +5718,7 @@
         <v>121.26828892653627</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="53" t="s">
         <v>172</v>
       </c>
@@ -5779,7 +5744,7 @@
         <v>121.26828892653627</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="53" t="s">
         <v>173</v>
       </c>
@@ -5805,7 +5770,7 @@
         <v>121.26828892653627</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="68" t="s">
         <v>98</v>
       </c>
@@ -5819,7 +5784,7 @@
       <c r="I86" s="17"/>
       <c r="J86" s="69"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="53" t="s">
         <v>174</v>
       </c>
@@ -5836,7 +5801,7 @@
         <v>121.26828892653627</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="37" t="s">
         <v>92</v>
       </c>
@@ -5871,12 +5836,12 @@
         <v>121.26828892653627</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="60" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="59" t="s">
         <v>117</v>
       </c>
@@ -5908,7 +5873,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="43" t="s">
         <v>92</v>
       </c>
@@ -5939,7 +5904,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="68" t="s">
         <v>98</v>
       </c>
@@ -5953,7 +5918,7 @@
       <c r="I95" s="17"/>
       <c r="J95" s="69"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="36" t="s">
         <v>116</v>
       </c>
@@ -5980,7 +5945,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="36" t="s">
         <v>118</v>
       </c>
@@ -6007,7 +5972,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="36" t="s">
         <v>119</v>
       </c>
@@ -6034,7 +5999,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="99" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="47" t="s">
         <v>120</v>
       </c>
@@ -6063,8 +6028,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="100" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="59" t="s">
         <v>123</v>
       </c>
@@ -6097,7 +6062,7 @@
       </c>
       <c r="K101" s="22"/>
     </row>
-    <row r="102" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="37" t="s">
         <v>92</v>
       </c>
@@ -6127,7 +6092,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="105" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="13" t="s">
         <v>53</v>
       </c>
@@ -6135,7 +6100,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="61" t="s">
         <v>124</v>
       </c>
@@ -6167,7 +6132,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="42" t="s">
         <v>54</v>
       </c>
@@ -6201,7 +6166,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="42" t="s">
         <v>55</v>
       </c>
@@ -6235,7 +6200,7 @@
         <v>0.16200000000000001</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="43" t="s">
         <v>92</v>
       </c>
@@ -6271,7 +6236,7 @@
         <v>27.882482758620689</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="68" t="s">
         <v>98</v>
       </c>
@@ -6285,7 +6250,7 @@
       <c r="I110" s="17"/>
       <c r="J110" s="69"/>
     </row>
-    <row r="111" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="47" t="s">
         <v>125</v>
       </c>
@@ -6307,12 +6272,12 @@
         <v>27.882482758620689</v>
       </c>
     </row>
-    <row r="114" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" s="30" t="s">
         <v>127</v>
       </c>
@@ -6345,7 +6310,7 @@
       </c>
       <c r="L115" s="22"/>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" s="34" t="s">
         <v>128</v>
       </c>
@@ -6379,13 +6344,13 @@
       </c>
       <c r="L116" s="7"/>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" s="36" t="s">
         <v>130</v>
       </c>
       <c r="J117" s="35"/>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" s="62" t="s">
         <v>131</v>
       </c>
@@ -6418,7 +6383,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="62" t="s">
         <v>132</v>
       </c>
@@ -6451,7 +6416,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" s="62" t="s">
         <v>133</v>
       </c>
@@ -6484,7 +6449,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" s="62" t="s">
         <v>134</v>
       </c>
@@ -6517,7 +6482,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" s="62" t="s">
         <v>129</v>
       </c>
@@ -6550,7 +6515,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" s="62" t="s">
         <v>135</v>
       </c>
@@ -6583,7 +6548,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124" s="70" t="s">
         <v>252</v>
       </c>
@@ -6618,7 +6583,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" s="71" t="s">
         <v>51</v>
       </c>
@@ -6642,7 +6607,7 @@
       <c r="I125" s="73"/>
       <c r="J125" s="74"/>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126" s="62" t="s">
         <v>255</v>
       </c>
@@ -6666,7 +6631,7 @@
       <c r="I126" s="73"/>
       <c r="J126" s="74"/>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="62" t="s">
         <v>251</v>
       </c>
@@ -6698,7 +6663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" s="62" t="s">
         <v>254</v>
       </c>
@@ -6730,7 +6695,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129" s="62" t="s">
         <v>253</v>
       </c>
@@ -6762,7 +6727,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="130" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="37" t="s">
         <v>92</v>
       </c>
@@ -6788,17 +6753,17 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131" s="3"/>
       <c r="C131" s="3"/>
     </row>
-    <row r="132" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>27</v>
       </c>
       <c r="F132" s="3"/>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A133" s="61" t="s">
         <v>175</v>
       </c>
@@ -6831,7 +6796,7 @@
       </c>
       <c r="L133" s="22"/>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A134" s="42" t="s">
         <v>176</v>
       </c>
@@ -6866,7 +6831,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135" s="42" t="s">
         <v>177</v>
       </c>
@@ -6900,7 +6865,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136" s="55" t="s">
         <v>178</v>
       </c>
@@ -6934,7 +6899,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137" s="43" t="s">
         <v>92</v>
       </c>
@@ -6971,7 +6936,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A138" s="68" t="s">
         <v>98</v>
       </c>
@@ -6985,7 +6950,7 @@
       <c r="I138" s="17"/>
       <c r="J138" s="69"/>
     </row>
-    <row r="139" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="63" t="s">
         <v>179</v>
       </c>
@@ -7014,19 +6979,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P84"/>
   <sheetViews>
     <sheetView topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A62" sqref="A62:B66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>136</v>
       </c>
@@ -7041,7 +7006,7 @@
       <c r="G1" s="14"/>
       <c r="H1" s="14"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>54</v>
       </c>
@@ -7061,7 +7026,7 @@
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>55</v>
       </c>
@@ -7081,7 +7046,7 @@
       <c r="G3" s="14"/>
       <c r="H3" s="14"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>92</v>
       </c>
@@ -7089,7 +7054,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>138</v>
       </c>
@@ -7097,7 +7062,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>140</v>
       </c>
@@ -7105,7 +7070,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>142</v>
       </c>
@@ -7113,7 +7078,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>143</v>
       </c>
@@ -7121,7 +7086,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>149</v>
       </c>
@@ -7129,7 +7094,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>148</v>
       </c>
@@ -7137,7 +7102,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>163</v>
       </c>
@@ -7145,7 +7110,7 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>164</v>
       </c>
@@ -7153,7 +7118,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>165</v>
       </c>
@@ -7161,7 +7126,7 @@
         <v>11.2</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>166</v>
       </c>
@@ -7169,7 +7134,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>182</v>
       </c>
@@ -7177,7 +7142,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>183</v>
       </c>
@@ -7201,7 +7166,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>185</v>
       </c>
@@ -7219,7 +7184,7 @@
         <v>1.44</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>186</v>
       </c>
@@ -7237,12 +7202,12 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>183</v>
       </c>
@@ -7260,7 +7225,7 @@
         <v>0.21000000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>185</v>
       </c>
@@ -7278,7 +7243,7 @@
         <v>0.30000000000000004</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>185</v>
       </c>
@@ -7296,7 +7261,7 @@
         <v>1.47</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>186</v>
       </c>
@@ -7314,12 +7279,12 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>183</v>
       </c>
@@ -7337,7 +7302,7 @@
         <v>0.21000000000000002</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>185</v>
       </c>
@@ -7355,7 +7320,7 @@
         <v>1.77</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>186</v>
       </c>
@@ -7373,7 +7338,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>64</v>
       </c>
@@ -7381,7 +7346,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>193</v>
       </c>
@@ -7399,7 +7364,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>185</v>
       </c>
@@ -7417,7 +7382,7 @@
         <v>1.51</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>186</v>
       </c>
@@ -7435,12 +7400,12 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>185</v>
       </c>
@@ -7459,7 +7424,7 @@
       </c>
       <c r="G47" s="3"/>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>193</v>
       </c>
@@ -7477,7 +7442,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>186</v>
       </c>
@@ -7495,12 +7460,12 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>185</v>
       </c>
@@ -7518,7 +7483,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>193</v>
       </c>
@@ -7539,7 +7504,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>186</v>
       </c>
@@ -7563,7 +7528,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H55">
         <v>24.88</v>
       </c>
@@ -7580,7 +7545,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>222</v>
       </c>
@@ -7603,7 +7568,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>193</v>
       </c>
@@ -7624,7 +7589,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>217</v>
       </c>
@@ -7645,7 +7610,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>186</v>
       </c>
@@ -7664,12 +7629,12 @@
       </c>
       <c r="F59" s="3"/>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>217</v>
       </c>
@@ -7678,7 +7643,7 @@
         <v>0.254</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>185</v>
       </c>
@@ -7687,7 +7652,7 @@
         <v>1.1200000000000001</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>193</v>
       </c>
@@ -7696,7 +7661,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>186</v>
       </c>
@@ -7705,12 +7670,12 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>217</v>
       </c>
@@ -7728,7 +7693,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>193</v>
       </c>
@@ -7746,7 +7711,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>186</v>
       </c>
@@ -7764,12 +7729,12 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>185</v>
       </c>
@@ -7787,7 +7752,7 @@
         <v>0.84000000000000008</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>193</v>
       </c>
@@ -7805,7 +7770,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>186</v>
       </c>
@@ -7823,12 +7788,12 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>185</v>
       </c>
@@ -7837,7 +7802,7 @@
         <v>0.84000000000000008</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>217</v>
       </c>
@@ -7846,7 +7811,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>193</v>
       </c>
@@ -7855,7 +7820,7 @@
         <v>0.21000000000000002</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>186</v>
       </c>
@@ -7871,29 +7836,29 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" customWidth="1"/>
-    <col min="8" max="8" width="14.5546875" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" customWidth="1"/>
-    <col min="10" max="10" width="25.44140625" customWidth="1"/>
-    <col min="11" max="11" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="25.42578125" customWidth="1"/>
+    <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -7925,7 +7890,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>88</v>
       </c>
@@ -7938,7 +7903,7 @@
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>43</v>
       </c>
@@ -7971,7 +7936,7 @@
       </c>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>74</v>
       </c>
@@ -8006,7 +7971,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>155</v>
       </c>
@@ -8042,7 +8007,7 @@
       </c>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>76</v>
       </c>
@@ -8077,7 +8042,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>77</v>
       </c>
@@ -8112,7 +8077,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>78</v>
       </c>
@@ -8147,7 +8112,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>75</v>
       </c>
@@ -8182,7 +8147,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>84</v>
       </c>
@@ -8213,7 +8178,7 @@
       </c>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>29</v>
       </c>
@@ -8227,7 +8192,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>80</v>
       </c>
@@ -8260,7 +8225,7 @@
       </c>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>79</v>
       </c>
@@ -8293,7 +8258,7 @@
       </c>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>45</v>
       </c>
@@ -8326,7 +8291,7 @@
       </c>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>46</v>
       </c>
@@ -8359,12 +8324,12 @@
       </c>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>41</v>
       </c>
@@ -8387,7 +8352,7 @@
       </c>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>42</v>
       </c>
@@ -8420,7 +8385,7 @@
       </c>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>16</v>
       </c>
@@ -8453,12 +8418,12 @@
       </c>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>145</v>
       </c>
@@ -8475,7 +8440,7 @@
       </c>
       <c r="J21" s="5"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>54</v>
       </c>
@@ -8503,7 +8468,7 @@
       </c>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>55</v>
       </c>
@@ -8531,7 +8496,7 @@
       </c>
       <c r="J23" s="5"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>92</v>
       </c>
@@ -8553,12 +8518,12 @@
       </c>
       <c r="J24" s="5"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>28</v>
       </c>
@@ -8572,7 +8537,7 @@
       <c r="I26" s="17"/>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
         <v>44</v>
       </c>
@@ -8603,7 +8568,7 @@
       </c>
       <c r="J27" s="5"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>47</v>
       </c>
@@ -8617,7 +8582,7 @@
       <c r="I28" s="19"/>
       <c r="J28" s="5"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
         <v>35</v>
       </c>
@@ -8651,7 +8616,7 @@
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
         <v>36</v>
       </c>
@@ -8685,7 +8650,7 @@
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
         <v>37</v>
       </c>
@@ -8721,7 +8686,7 @@
       </c>
       <c r="K31" s="5"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
         <v>57</v>
       </c>
@@ -8755,7 +8720,7 @@
       </c>
       <c r="J32" s="5"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
         <v>27</v>
       </c>
@@ -8772,7 +8737,7 @@
       </c>
       <c r="J33" s="5"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
         <v>38</v>
       </c>
@@ -8805,7 +8770,7 @@
       </c>
       <c r="J34" s="5"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
         <v>39</v>
       </c>
@@ -8839,7 +8804,7 @@
       <c r="J35" s="5"/>
       <c r="K35" s="5"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
         <v>40</v>
       </c>
@@ -8873,7 +8838,7 @@
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="18"/>
       <c r="B37" s="18"/>
       <c r="C37" s="17"/>
@@ -8889,12 +8854,12 @@
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="J38" s="20"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="24" t="s">
         <v>92</v>
       </c>
@@ -8914,7 +8879,7 @@
       </c>
       <c r="J39" s="20"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H40" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
User Defined Conductors Defined
Conductor paths from NGTN to PCB faces have been added. Also included in the thermal properties excel. Determined by a rough estimation using AI.
</commit_message>
<xml_diff>
--- a/PoCat3_Thermal_Model_Mass_Properties.xlsx
+++ b/PoCat3_Thermal_Model_Mass_Properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oscar\Documents\GitHub\PoCat-Thermal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8041057C-619F-47FC-B322-1D5207889C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F7EC71-4B3C-4EE5-BD19-575C5C3DBEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="48" yWindow="36" windowWidth="22992" windowHeight="12324" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Materials" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="379">
   <si>
     <t>Material</t>
   </si>
@@ -906,9 +906,6 @@
     <t>Conductance G (W/K)</t>
   </si>
   <si>
-    <t>RθJC​ (°C/W)</t>
-  </si>
-  <si>
     <t>Component</t>
   </si>
   <si>
@@ -1045,13 +1042,157 @@
   </si>
   <si>
     <t>HMC358MS8GE</t>
+  </si>
+  <si>
+    <t>Package Type</t>
+  </si>
+  <si>
+    <t>ΘJA (°C/W)</t>
+  </si>
+  <si>
+    <t>ΘJB (°C/W)</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>10–20</t>
+  </si>
+  <si>
+    <t>Small plastic package; primary heat path through PCB.</t>
+  </si>
+  <si>
+    <t>5–15</t>
+  </si>
+  <si>
+    <t>SQFN016V4040 (4x4 mm)</t>
+  </si>
+  <si>
+    <t>5–10</t>
+  </si>
+  <si>
+    <t>100–150</t>
+  </si>
+  <si>
+    <t>Exposed pad enhances thermal performance.</t>
+  </si>
+  <si>
+    <t>Thin QFN with efficient heat dissipation.</t>
+  </si>
+  <si>
+    <t>120–180</t>
+  </si>
+  <si>
+    <t>10–15</t>
+  </si>
+  <si>
+    <t>Exposed pad directs heat to PCB.</t>
+  </si>
+  <si>
+    <t>LQFP-64</t>
+  </si>
+  <si>
+    <t>Larger package; better heat spreading.</t>
+  </si>
+  <si>
+    <t>Generic SMT; assume plastic package.</t>
+  </si>
+  <si>
+    <t>Leadless QFN with exposed pad.</t>
+  </si>
+  <si>
+    <t>Standard QFN thermal performance.</t>
+  </si>
+  <si>
+    <t>2–5</t>
+  </si>
+  <si>
+    <t>Larger package; better heat transfer.</t>
+  </si>
+  <si>
+    <t>Exposed pad for PCB heat transfer.</t>
+  </si>
+  <si>
+    <t>Tiny package (2x2mm); limited thermal paths.</t>
+  </si>
+  <si>
+    <t>Similar to TSSOP; plastic encapsulation.</t>
+  </si>
+  <si>
+    <t>60–120</t>
+  </si>
+  <si>
+    <t>Exposed pad benefits from 2s2p PCB.</t>
+  </si>
+  <si>
+    <t>80–120</t>
+  </si>
+  <si>
+    <t>Similar to QFN; benefits from 2s2p PCB.</t>
+  </si>
+  <si>
+    <t>40–80</t>
+  </si>
+  <si>
+    <t>Limited improvement due to plastic package.</t>
+  </si>
+  <si>
+    <t>Likely QFN; benefits from 2s2p PCB.</t>
+  </si>
+  <si>
+    <t>40–60</t>
+  </si>
+  <si>
+    <t>Moderate improvement in ΘJAΘJA​.</t>
+  </si>
+  <si>
+    <t>Improved ΘJAΘJA​ due to better heat spreading.</t>
+  </si>
+  <si>
+    <t>Exposed pad for low ΘJBΘJB​.</t>
+  </si>
+  <si>
+    <t>ΘJB1 (°C/W)</t>
+  </si>
+  <si>
+    <t>ΘJB2 (°C/W)</t>
+  </si>
+  <si>
+    <t>ΘJBEst (°C/W)</t>
+  </si>
+  <si>
+    <t>https://www.ti.com/lit/an/spra953d/spra953d.pdf?ts=1742435438606</t>
+  </si>
+  <si>
+    <t>https://www.analog.com/en/resources/technical-articles/thermal-characterization-of-ic-packages.html</t>
+  </si>
+  <si>
+    <t>https://fscdn.rohm.com/en/products/databook/applinote/common/how_to_use_the_rth_and_thermal_characteristics_parameters_an-e.pdf</t>
+  </si>
+  <si>
+    <t>Theory</t>
+  </si>
+  <si>
+    <t>Estimations using AI</t>
+  </si>
+  <si>
+    <t>Estimation 2</t>
+  </si>
+  <si>
+    <t>The highest resistance provided has been chosen, between the two of them.</t>
+  </si>
+  <si>
+    <t>Determining Theta_JB requieres extensive testing, not possible nor necessary.</t>
+  </si>
+  <si>
+    <t>UDC=User Defined Conductor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1116,6 +1257,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1358,7 +1506,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1495,6 +1643,20 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
@@ -1602,55 +1764,6 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>726141</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>681317</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>8415</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95EABFAC-BF3B-4CC8-9045-976DB304130F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7862047" y="0"/>
-          <a:ext cx="4688541" cy="2339239"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -4241,7 +4354,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L139"/>
   <sheetViews>
-    <sheetView topLeftCell="A74" zoomScale="68" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C126" sqref="C126"/>
     </sheetView>
   </sheetViews>
@@ -7325,30 +7438,33 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40D53AE0-DA50-4BFF-91F5-0F83D06C1B07}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.109375" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.44140625" customWidth="1"/>
+    <col min="6" max="6" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5546875" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="56.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C1" s="75" t="s">
         <v>261</v>
@@ -7362,19 +7478,29 @@
       <c r="F1" s="75" t="s">
         <v>264</v>
       </c>
-      <c r="G1" s="75" t="s">
-        <v>285</v>
-      </c>
-      <c r="H1" s="75" t="s">
+      <c r="G1" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="J1" s="75" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L1" s="82" t="s">
+        <v>378</v>
+      </c>
+      <c r="M1" s="82"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B2" s="77" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>265</v>
@@ -7388,19 +7514,26 @@
       <c r="F2" s="5">
         <v>0.45</v>
       </c>
-      <c r="G2" s="29">
+      <c r="G2" s="5">
         <v>20</v>
       </c>
-      <c r="H2" s="29">
+      <c r="H2" t="s">
+        <v>335</v>
+      </c>
+      <c r="I2" s="29">
+        <v>20</v>
+      </c>
+      <c r="J2" s="78">
+        <f>1/G2</f>
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B3" s="77" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>265</v>
@@ -7414,19 +7547,26 @@
       <c r="F3" s="5">
         <v>0.45</v>
       </c>
-      <c r="G3" s="29">
+      <c r="G3" s="5">
         <v>20</v>
       </c>
-      <c r="H3" s="29">
+      <c r="H3" t="s">
+        <v>335</v>
+      </c>
+      <c r="I3" s="29">
+        <v>20</v>
+      </c>
+      <c r="J3" s="78">
+        <f t="shared" ref="J3:J26" si="0">1/G3</f>
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B4" s="77" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>265</v>
@@ -7440,19 +7580,29 @@
       <c r="F4" s="5">
         <v>0.45</v>
       </c>
-      <c r="G4" s="29">
+      <c r="G4" s="5">
         <v>20</v>
       </c>
-      <c r="H4" s="29">
+      <c r="H4" t="s">
+        <v>335</v>
+      </c>
+      <c r="I4" s="29">
+        <v>20</v>
+      </c>
+      <c r="J4" s="78">
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L4" s="2" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>266</v>
@@ -7466,19 +7616,29 @@
       <c r="F5" s="5">
         <v>0.91</v>
       </c>
-      <c r="G5" s="29">
+      <c r="G5" s="5">
         <v>15</v>
       </c>
-      <c r="H5" s="29">
-        <v>6.7000000000000004E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H5" t="s">
+        <v>337</v>
+      </c>
+      <c r="I5" s="29">
+        <v>15</v>
+      </c>
+      <c r="J5" s="78">
+        <f t="shared" si="0"/>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="L5" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B6" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>267</v>
@@ -7492,19 +7652,29 @@
       <c r="F6" s="5">
         <v>1</v>
       </c>
-      <c r="G6" s="29">
+      <c r="G6" s="5">
         <v>4</v>
       </c>
-      <c r="H6" s="29">
+      <c r="H6" t="s">
+        <v>339</v>
+      </c>
+      <c r="I6" s="29">
+        <v>10</v>
+      </c>
+      <c r="J6" s="78">
+        <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L6" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B7" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>268</v>
@@ -7518,19 +7688,29 @@
       <c r="F7" s="5">
         <v>0.5</v>
       </c>
-      <c r="G7" s="29">
+      <c r="G7" s="5">
         <v>5</v>
       </c>
-      <c r="H7" s="29">
+      <c r="H7" t="s">
+        <v>339</v>
+      </c>
+      <c r="I7" s="29">
+        <v>10</v>
+      </c>
+      <c r="J7" s="78">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L7" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>269</v>
@@ -7544,16 +7724,26 @@
       <c r="F8" s="5">
         <v>1</v>
       </c>
-      <c r="G8" s="29">
+      <c r="G8" s="5">
         <v>15</v>
       </c>
-      <c r="H8" s="29">
-        <v>6.7000000000000004E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H8" t="s">
+        <v>335</v>
+      </c>
+      <c r="I8" s="29">
+        <v>20</v>
+      </c>
+      <c r="J8" s="78">
+        <f t="shared" si="0"/>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="L8" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="76" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B9" s="76"/>
       <c r="C9" s="76"/>
@@ -7562,13 +7752,15 @@
       <c r="F9" s="76"/>
       <c r="G9" s="76"/>
       <c r="H9" s="76"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9" s="79"/>
+      <c r="J9" s="76"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B10" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>270</v>
@@ -7582,19 +7774,26 @@
       <c r="F10" s="5">
         <v>0.5</v>
       </c>
-      <c r="G10" s="29">
+      <c r="G10" s="5">
         <v>7</v>
       </c>
-      <c r="H10" s="29">
-        <v>0.14299999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H10" t="s">
+        <v>339</v>
+      </c>
+      <c r="I10" s="29">
+        <v>10</v>
+      </c>
+      <c r="J10" s="78">
+        <f t="shared" si="0"/>
+        <v>0.14285714285714285</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B11" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>271</v>
@@ -7608,19 +7807,29 @@
       <c r="F11" s="5">
         <v>0.5</v>
       </c>
-      <c r="G11" s="29">
+      <c r="G11" s="5">
         <v>7</v>
       </c>
-      <c r="H11" s="29">
-        <v>0.14299999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H11" t="s">
+        <v>339</v>
+      </c>
+      <c r="I11" s="29">
+        <v>10</v>
+      </c>
+      <c r="J11" s="78">
+        <f t="shared" si="0"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="L11" s="80" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B12" s="77" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>272</v>
@@ -7634,19 +7843,32 @@
       <c r="F12" s="5">
         <v>0.5</v>
       </c>
-      <c r="G12" s="29">
+      <c r="G12" s="5">
         <v>20</v>
       </c>
-      <c r="H12" s="29">
+      <c r="H12" t="s">
+        <v>344</v>
+      </c>
+      <c r="I12" s="29">
+        <v>20</v>
+      </c>
+      <c r="J12" s="78">
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L12" s="81" t="s">
+        <v>376</v>
+      </c>
+      <c r="M12" s="81"/>
+      <c r="N12" s="81"/>
+      <c r="O12" s="81"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B13" s="77" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>272</v>
@@ -7660,19 +7882,30 @@
       <c r="F13" s="5">
         <v>0.5</v>
       </c>
-      <c r="G13" s="29">
+      <c r="G13" s="5">
         <v>20</v>
       </c>
-      <c r="H13" s="29">
+      <c r="H13" t="s">
+        <v>344</v>
+      </c>
+      <c r="I13" s="29">
+        <v>20</v>
+      </c>
+      <c r="J13" s="78">
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L13" s="81"/>
+      <c r="M13" s="81"/>
+      <c r="N13" s="81"/>
+      <c r="O13" s="81"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B14" s="77" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>272</v>
@@ -7686,19 +7919,32 @@
       <c r="F14" s="5">
         <v>0.5</v>
       </c>
-      <c r="G14" s="29">
+      <c r="G14" s="5">
         <v>20</v>
       </c>
-      <c r="H14" s="29">
+      <c r="H14" t="s">
+        <v>344</v>
+      </c>
+      <c r="I14" s="29">
+        <v>20</v>
+      </c>
+      <c r="J14" s="78">
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L14" s="83" t="s">
+        <v>377</v>
+      </c>
+      <c r="M14" s="81"/>
+      <c r="N14" s="81"/>
+      <c r="O14" s="81"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B15" s="77" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>273</v>
@@ -7712,71 +7958,99 @@
       <c r="F15" s="5">
         <v>0.75</v>
       </c>
-      <c r="G15" s="29">
+      <c r="G15" s="5">
         <v>3</v>
       </c>
-      <c r="H15" s="29">
-        <v>0.33300000000000002</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>301</v>
-      </c>
-      <c r="B16" s="77" t="s">
-        <v>322</v>
-      </c>
-      <c r="C16" s="5" t="s">
+      <c r="H15" t="s">
+        <v>339</v>
+      </c>
+      <c r="I15" s="29">
+        <v>10</v>
+      </c>
+      <c r="J15" s="78">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="L15" s="83"/>
+    </row>
+    <row r="16" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="C16" s="29" t="s">
         <v>274</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="29">
         <v>10</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="29">
         <v>10</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="29">
         <v>1.6</v>
       </c>
       <c r="G16" s="29">
         <v>10</v>
       </c>
-      <c r="H16" s="29">
+      <c r="H16" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="I16" s="29">
+        <v>15</v>
+      </c>
+      <c r="J16" s="78">
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>302</v>
-      </c>
-      <c r="B17" s="77" t="s">
-        <v>323</v>
-      </c>
-      <c r="C17" s="5" t="s">
+      <c r="M16" s="81"/>
+      <c r="N16" s="81"/>
+      <c r="O16" s="81"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="C17" s="29" t="s">
         <v>275</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="29">
         <v>4</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="29">
         <v>4</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="29">
         <v>0.5</v>
       </c>
       <c r="G17" s="29">
         <v>4</v>
       </c>
-      <c r="H17" s="29">
+      <c r="H17" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="I17" s="29">
+        <v>10</v>
+      </c>
+      <c r="J17" s="78">
+        <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="M17" s="81"/>
+      <c r="N17" s="81"/>
+      <c r="O17" s="81"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B18" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>276</v>
@@ -7790,19 +8064,30 @@
       <c r="F18" s="5">
         <v>0.5</v>
       </c>
-      <c r="G18" s="29">
+      <c r="G18" s="5">
         <v>5</v>
       </c>
-      <c r="H18" s="29">
+      <c r="H18" t="s">
+        <v>335</v>
+      </c>
+      <c r="I18" s="29">
+        <v>20</v>
+      </c>
+      <c r="J18" s="78">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L18" s="81"/>
+      <c r="M18" s="81"/>
+      <c r="N18" s="81"/>
+      <c r="O18" s="81"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B19" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>277</v>
@@ -7816,19 +8101,26 @@
       <c r="F19" s="5">
         <v>0.5</v>
       </c>
-      <c r="G19" s="29">
+      <c r="G19" s="5">
         <v>5</v>
       </c>
-      <c r="H19" s="29">
+      <c r="H19" t="s">
+        <v>339</v>
+      </c>
+      <c r="I19" s="29">
+        <v>10</v>
+      </c>
+      <c r="J19" s="78">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B20" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>278</v>
@@ -7842,19 +8134,26 @@
       <c r="F20" s="5">
         <v>0.5</v>
       </c>
-      <c r="G20" s="29">
+      <c r="G20" s="5">
         <v>4</v>
       </c>
-      <c r="H20" s="29">
+      <c r="H20" t="s">
+        <v>339</v>
+      </c>
+      <c r="I20" s="29">
+        <v>10</v>
+      </c>
+      <c r="J20" s="78">
+        <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B21" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>279</v>
@@ -7868,19 +8167,26 @@
       <c r="F21" s="5">
         <v>0.5</v>
       </c>
-      <c r="G21" s="29">
+      <c r="G21" s="5">
         <v>5</v>
       </c>
-      <c r="H21" s="29">
+      <c r="H21" t="s">
+        <v>339</v>
+      </c>
+      <c r="I21" s="29">
+        <v>10</v>
+      </c>
+      <c r="J21" s="78">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B22" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>280</v>
@@ -7894,19 +8200,26 @@
       <c r="F22" s="5">
         <v>2.0299999999999998</v>
       </c>
-      <c r="G22" s="29">
+      <c r="G22" s="5">
         <v>8</v>
       </c>
-      <c r="H22" s="29">
+      <c r="H22" t="s">
+        <v>351</v>
+      </c>
+      <c r="I22" s="29">
+        <v>5</v>
+      </c>
+      <c r="J22" s="78">
+        <f t="shared" si="0"/>
         <v>0.125</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B23" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>281</v>
@@ -7920,19 +8233,26 @@
       <c r="F23" s="5">
         <v>0.5</v>
       </c>
-      <c r="G23" s="29">
+      <c r="G23" s="5">
         <v>7</v>
       </c>
-      <c r="H23" s="29">
-        <v>0.14299999999999999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H23" t="s">
+        <v>339</v>
+      </c>
+      <c r="I23" s="29">
+        <v>10</v>
+      </c>
+      <c r="J23" s="78">
+        <f t="shared" si="0"/>
+        <v>0.14285714285714285</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B24" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>282</v>
@@ -7946,19 +8266,26 @@
       <c r="F24" s="5">
         <v>0.89</v>
       </c>
-      <c r="G24" s="29">
+      <c r="G24" s="5">
         <v>10</v>
       </c>
-      <c r="H24" s="29">
+      <c r="H24" t="s">
+        <v>335</v>
+      </c>
+      <c r="I24" s="29">
+        <v>20</v>
+      </c>
+      <c r="J24" s="78">
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B25" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>282</v>
@@ -7972,19 +8299,26 @@
       <c r="F25" s="5">
         <v>0.89</v>
       </c>
-      <c r="G25" s="29">
+      <c r="G25" s="5">
         <v>10</v>
       </c>
-      <c r="H25" s="29">
+      <c r="H25" t="s">
+        <v>335</v>
+      </c>
+      <c r="I25" s="29">
+        <v>20</v>
+      </c>
+      <c r="J25" s="78">
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B26" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>283</v>
@@ -7998,16 +8332,532 @@
       <c r="F26" s="5">
         <v>0.5</v>
       </c>
-      <c r="G26" s="29">
+      <c r="G26" s="5">
         <v>20</v>
       </c>
-      <c r="H26" s="29">
+      <c r="H26" t="s">
+        <v>344</v>
+      </c>
+      <c r="I26" s="29">
+        <v>15</v>
+      </c>
+      <c r="J26" s="78">
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
     </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>375</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="L30" s="75" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F31" s="2"/>
+      <c r="K31" t="s">
+        <v>265</v>
+      </c>
+      <c r="L31" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>312</v>
+      </c>
+      <c r="B32" t="s">
+        <v>265</v>
+      </c>
+      <c r="C32" t="s">
+        <v>343</v>
+      </c>
+      <c r="D32" t="s">
+        <v>335</v>
+      </c>
+      <c r="K32" t="s">
+        <v>265</v>
+      </c>
+      <c r="L32" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>312</v>
+      </c>
+      <c r="B33" t="s">
+        <v>265</v>
+      </c>
+      <c r="C33" t="s">
+        <v>343</v>
+      </c>
+      <c r="D33" t="s">
+        <v>335</v>
+      </c>
+      <c r="K33" t="s">
+        <v>265</v>
+      </c>
+      <c r="L33" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>312</v>
+      </c>
+      <c r="B34" t="s">
+        <v>265</v>
+      </c>
+      <c r="C34" t="s">
+        <v>343</v>
+      </c>
+      <c r="D34" t="s">
+        <v>335</v>
+      </c>
+      <c r="K34" t="s">
+        <v>266</v>
+      </c>
+      <c r="L34" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>313</v>
+      </c>
+      <c r="B35" t="s">
+        <v>266</v>
+      </c>
+      <c r="C35" t="s">
+        <v>356</v>
+      </c>
+      <c r="D35" t="s">
+        <v>337</v>
+      </c>
+      <c r="K35" t="s">
+        <v>338</v>
+      </c>
+      <c r="L35" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>314</v>
+      </c>
+      <c r="B36" t="s">
+        <v>338</v>
+      </c>
+      <c r="C36" t="s">
+        <v>356</v>
+      </c>
+      <c r="D36" t="s">
+        <v>339</v>
+      </c>
+      <c r="K36" t="s">
+        <v>268</v>
+      </c>
+      <c r="L36" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>315</v>
+      </c>
+      <c r="B37" t="s">
+        <v>268</v>
+      </c>
+      <c r="C37" t="s">
+        <v>356</v>
+      </c>
+      <c r="D37" t="s">
+        <v>339</v>
+      </c>
+      <c r="K37" t="s">
+        <v>269</v>
+      </c>
+      <c r="L37" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>316</v>
+      </c>
+      <c r="B38" t="s">
+        <v>269</v>
+      </c>
+      <c r="C38" t="s">
+        <v>358</v>
+      </c>
+      <c r="D38" t="s">
+        <v>335</v>
+      </c>
+      <c r="K38" t="s">
+        <v>270</v>
+      </c>
+      <c r="L38" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>317</v>
+      </c>
+      <c r="B39" t="s">
+        <v>270</v>
+      </c>
+      <c r="C39" t="s">
+        <v>358</v>
+      </c>
+      <c r="D39" t="s">
+        <v>339</v>
+      </c>
+      <c r="K39" t="s">
+        <v>271</v>
+      </c>
+      <c r="L39" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>318</v>
+      </c>
+      <c r="B40" t="s">
+        <v>271</v>
+      </c>
+      <c r="C40" t="s">
+        <v>360</v>
+      </c>
+      <c r="D40" t="s">
+        <v>339</v>
+      </c>
+      <c r="K40" t="s">
+        <v>272</v>
+      </c>
+      <c r="L40" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>319</v>
+      </c>
+      <c r="B41" t="s">
+        <v>272</v>
+      </c>
+      <c r="C41" t="s">
+        <v>340</v>
+      </c>
+      <c r="D41" t="s">
+        <v>344</v>
+      </c>
+      <c r="K41" t="s">
+        <v>272</v>
+      </c>
+      <c r="L41" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>319</v>
+      </c>
+      <c r="B42" t="s">
+        <v>272</v>
+      </c>
+      <c r="C42" t="s">
+        <v>340</v>
+      </c>
+      <c r="D42" t="s">
+        <v>344</v>
+      </c>
+      <c r="K42" t="s">
+        <v>272</v>
+      </c>
+      <c r="L42" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>319</v>
+      </c>
+      <c r="B43" t="s">
+        <v>272</v>
+      </c>
+      <c r="C43" t="s">
+        <v>340</v>
+      </c>
+      <c r="D43" t="s">
+        <v>344</v>
+      </c>
+      <c r="K43" t="s">
+        <v>273</v>
+      </c>
+      <c r="L43" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>320</v>
+      </c>
+      <c r="B44" t="s">
+        <v>273</v>
+      </c>
+      <c r="C44" t="s">
+        <v>356</v>
+      </c>
+      <c r="D44" t="s">
+        <v>339</v>
+      </c>
+      <c r="K44" t="s">
+        <v>346</v>
+      </c>
+      <c r="L44" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>321</v>
+      </c>
+      <c r="B45" t="s">
+        <v>346</v>
+      </c>
+      <c r="C45" t="s">
+        <v>360</v>
+      </c>
+      <c r="D45" t="s">
+        <v>337</v>
+      </c>
+      <c r="K45" t="s">
+        <v>275</v>
+      </c>
+      <c r="L45" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>322</v>
+      </c>
+      <c r="B46" t="s">
+        <v>275</v>
+      </c>
+      <c r="C46" t="s">
+        <v>356</v>
+      </c>
+      <c r="D46" t="s">
+        <v>339</v>
+      </c>
+      <c r="K46" t="s">
+        <v>276</v>
+      </c>
+      <c r="L46" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>323</v>
+      </c>
+      <c r="B47" t="s">
+        <v>276</v>
+      </c>
+      <c r="C47" t="s">
+        <v>358</v>
+      </c>
+      <c r="D47" t="s">
+        <v>335</v>
+      </c>
+      <c r="K47" t="s">
+        <v>277</v>
+      </c>
+      <c r="L47" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>324</v>
+      </c>
+      <c r="B48" t="s">
+        <v>277</v>
+      </c>
+      <c r="C48" t="s">
+        <v>356</v>
+      </c>
+      <c r="D48" t="s">
+        <v>339</v>
+      </c>
+      <c r="K48" t="s">
+        <v>278</v>
+      </c>
+      <c r="L48" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>325</v>
+      </c>
+      <c r="B49" t="s">
+        <v>278</v>
+      </c>
+      <c r="C49" t="s">
+        <v>356</v>
+      </c>
+      <c r="D49" t="s">
+        <v>339</v>
+      </c>
+      <c r="K49" t="s">
+        <v>279</v>
+      </c>
+      <c r="L49" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>326</v>
+      </c>
+      <c r="B50" t="s">
+        <v>279</v>
+      </c>
+      <c r="C50" t="s">
+        <v>356</v>
+      </c>
+      <c r="D50" t="s">
+        <v>339</v>
+      </c>
+      <c r="K50" t="s">
+        <v>280</v>
+      </c>
+      <c r="L50" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>327</v>
+      </c>
+      <c r="B51" t="s">
+        <v>280</v>
+      </c>
+      <c r="C51" t="s">
+        <v>363</v>
+      </c>
+      <c r="D51" t="s">
+        <v>351</v>
+      </c>
+      <c r="K51" t="s">
+        <v>281</v>
+      </c>
+      <c r="L51" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>328</v>
+      </c>
+      <c r="B52" t="s">
+        <v>281</v>
+      </c>
+      <c r="C52" t="s">
+        <v>358</v>
+      </c>
+      <c r="D52" t="s">
+        <v>339</v>
+      </c>
+      <c r="K52" t="s">
+        <v>282</v>
+      </c>
+      <c r="L52" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>329</v>
+      </c>
+      <c r="B53" t="s">
+        <v>282</v>
+      </c>
+      <c r="C53" t="s">
+        <v>343</v>
+      </c>
+      <c r="D53" t="s">
+        <v>335</v>
+      </c>
+      <c r="K53" t="s">
+        <v>282</v>
+      </c>
+      <c r="L53" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>329</v>
+      </c>
+      <c r="B54" t="s">
+        <v>282</v>
+      </c>
+      <c r="C54" t="s">
+        <v>343</v>
+      </c>
+      <c r="D54" t="s">
+        <v>335</v>
+      </c>
+      <c r="K54" t="s">
+        <v>283</v>
+      </c>
+      <c r="L54" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>330</v>
+      </c>
+      <c r="B55" t="s">
+        <v>283</v>
+      </c>
+      <c r="C55" t="s">
+        <v>340</v>
+      </c>
+      <c r="D55" t="s">
+        <v>344</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="L14:L15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8016,7 +8866,7 @@
   <dimension ref="A1:P84"/>
   <sheetViews>
     <sheetView topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62:B66"/>
+      <selection activeCell="G64" sqref="G63:G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Conductive Interfaces First Version
Model Assembly, Conductive Interfaces added and renamed, geometry combined. Some interfaces are still missing while others are to be revisited.
</commit_message>
<xml_diff>
--- a/PoCat3_Thermal_Model_Mass_Properties.xlsx
+++ b/PoCat3_Thermal_Model_Mass_Properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oscar\Documents\GitHub\PoCat-Thermal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F7EC71-4B3C-4EE5-BD19-575C5C3DBEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31EF3367-98FA-47D3-845E-B530EEC4B176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48" yWindow="36" windowWidth="22992" windowHeight="12324" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Materials" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,9 @@
     <sheet name="Properties PCBs" sheetId="10" r:id="rId3"/>
     <sheet name="Bulks" sheetId="6" r:id="rId4"/>
     <sheet name="UDC" sheetId="11" r:id="rId5"/>
-    <sheet name="Extra" sheetId="9" r:id="rId6"/>
-    <sheet name="Masses and Volumes Old VC" sheetId="7" r:id="rId7"/>
+    <sheet name="Conductances" sheetId="12" r:id="rId6"/>
+    <sheet name="Extra" sheetId="9" r:id="rId7"/>
+    <sheet name="Masses and Volumes Old VC" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
@@ -7440,7 +7441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40D53AE0-DA50-4BFF-91F5-0F83D06C1B07}">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A21" sqref="A21:J21"/>
     </sheetView>
   </sheetViews>
@@ -8862,6 +8863,18 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22733B97-020B-4F8D-AA6D-CE76BADDD329}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:P84"/>
   <sheetViews>
@@ -9718,7 +9731,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:L40"/>
   <sheetViews>

</xml_diff>

<commit_message>
Small fix to MTQ density
</commit_message>
<xml_diff>
--- a/PoCat3_Thermal_Model_Mass_Properties.xlsx
+++ b/PoCat3_Thermal_Model_Mass_Properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oscar\Documents\GitHub\PoCat-Thermal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9F472D-5A90-450D-8238-3BB999897A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E127DD-0493-4395-8D7E-968546525D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Materials" sheetId="1" r:id="rId1"/>
@@ -1374,7 +1374,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1527,12 +1527,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1723,6 +1732,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
@@ -2736,7 +2747,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -4434,8 +4445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L139"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G135" sqref="G135"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5374,21 +5385,22 @@
       <c r="B40" t="s">
         <v>213</v>
       </c>
-      <c r="C40">
-        <v>7.1</v>
+      <c r="C40" s="110">
+        <v>6.6</v>
       </c>
       <c r="D40" s="69">
         <f>C40/1000</f>
-        <v>7.0999999999999995E-3</v>
+        <v>6.6E-3</v>
       </c>
       <c r="E40">
         <f>C40/C42</f>
-        <v>1.0757575757575757</v>
+        <v>0.92957746478873238</v>
       </c>
       <c r="F40" s="69" t="s">
         <v>23</v>
       </c>
       <c r="G40" s="84">
+        <f>D40/F42</f>
         <v>1629.6296296296296</v>
       </c>
       <c r="H40" s="84">
@@ -5409,15 +5421,15 @@
         <v>93</v>
       </c>
       <c r="C41">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D41" s="69">
         <f t="shared" ref="D41:D42" si="1">C41/1000</f>
-        <v>0</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="E41">
-        <f>C41/C42</f>
-        <v>0</v>
+        <f>C41/C40</f>
+        <v>7.575757575757576E-2</v>
       </c>
       <c r="F41" s="69" t="s">
         <v>23</v>
@@ -5442,20 +5454,19 @@
       <c r="B42" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="C42" s="36">
-        <v>6.6</v>
+      <c r="C42" s="111">
+        <v>7.1</v>
       </c>
       <c r="D42" s="70">
-        <f t="shared" si="1"/>
-        <v>6.6E-3</v>
+        <f>C42/1000</f>
+        <v>7.0999999999999995E-3</v>
       </c>
       <c r="E42" s="36"/>
       <c r="F42" s="70">
         <v>4.0500000000000002E-6</v>
       </c>
       <c r="G42" s="83">
-        <f>D40/F42</f>
-        <v>1753.0864197530861</v>
+        <v>1629.6296296296296</v>
       </c>
       <c r="H42" s="83">
         <v>903.96364021734939</v>
@@ -7775,7 +7786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Formatting on excel fixes
</commit_message>
<xml_diff>
--- a/PoCat3_Thermal_Model_Mass_Properties.xlsx
+++ b/PoCat3_Thermal_Model_Mass_Properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oscar\Documents\GitHub\PoCat-Thermal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE37FDCC-BB21-4CB9-8565-E2D0131E9E7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4072BD22-43B3-47F6-9841-6DF049D9F22D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48" yWindow="36" windowWidth="22992" windowHeight="12324" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="48" yWindow="36" windowWidth="22992" windowHeight="12324" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Materials" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1128" uniqueCount="386">
   <si>
     <t>Material</t>
   </si>
@@ -1541,7 +1541,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1724,6 +1724,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1733,7 +1734,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
@@ -2305,8 +2306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:F4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2747,8 +2748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3844,7 +3845,7 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4443,10 +4444,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:L139"/>
+  <dimension ref="A1:L138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+    <sheetView topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5598,7 +5599,7 @@
       <c r="A48" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="B48" s="111" t="s">
+      <c r="B48" s="108" t="s">
         <v>22</v>
       </c>
       <c r="C48" s="36">
@@ -6068,8 +6069,8 @@
       <c r="D68" s="68" t="s">
         <v>96</v>
       </c>
-      <c r="E68" s="31">
-        <v>1</v>
+      <c r="E68" s="31" t="s">
+        <v>94</v>
       </c>
       <c r="F68" s="68" t="s">
         <v>86</v>
@@ -6102,13 +6103,25 @@
         <f>C69/1000</f>
         <v>7.6E-3</v>
       </c>
+      <c r="E69" s="112">
+        <f>D69/D71</f>
+        <v>0.91566265060240981</v>
+      </c>
       <c r="F69" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="G69" s="84"/>
-      <c r="H69" s="84"/>
-      <c r="I69" s="72"/>
-      <c r="J69" s="96"/>
+      <c r="G69" s="84">
+        <v>3242.1874999999991</v>
+      </c>
+      <c r="H69" s="84">
+        <v>904.86619540520076</v>
+      </c>
+      <c r="I69" s="72">
+        <v>0.29142496305131627</v>
+      </c>
+      <c r="J69" s="96">
+        <v>88.525164000000032</v>
+      </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="38" t="s">
@@ -6121,258 +6134,281 @@
         <v>0.7</v>
       </c>
       <c r="D70" s="69">
-        <f t="shared" ref="D70:D72" si="2">C70/1000</f>
+        <f t="shared" ref="D70:D71" si="2">C70/1000</f>
         <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="E70" s="112">
+        <f>D70/D71</f>
+        <v>8.4337349397590383E-2</v>
       </c>
       <c r="F70" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="G70" s="84"/>
-      <c r="H70" s="84"/>
-      <c r="I70" s="72"/>
-      <c r="J70" s="96"/>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A71" s="38" t="s">
-        <v>91</v>
+      <c r="G70" s="84">
+        <v>3242.1874999999991</v>
+      </c>
+      <c r="H70" s="84">
+        <v>904.86619540520076</v>
+      </c>
+      <c r="I70" s="72">
+        <v>0.29142496305131627</v>
+      </c>
+      <c r="J70" s="96">
+        <v>88.525164000000032</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="B71" s="36"/>
+      <c r="C71" s="36">
+        <f>SUM(C69:C70)</f>
+        <v>8.2999999999999989</v>
       </c>
       <c r="D71" s="69">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F71" s="69" t="s">
+        <v>8.2999999999999984E-3</v>
+      </c>
+      <c r="E71" s="36"/>
+      <c r="F71" s="70">
+        <v>2.5600000000000001E-6</v>
+      </c>
+      <c r="G71" s="83">
+        <f>D71/F71</f>
+        <v>3242.1874999999991</v>
+      </c>
+      <c r="H71" s="83">
+        <v>904.86619540520076</v>
+      </c>
+      <c r="I71" s="75">
+        <v>0.29142496305131627</v>
+      </c>
+      <c r="J71" s="95">
+        <v>88.525164000000032</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="23"/>
+      <c r="D72" s="69"/>
+      <c r="F72" s="69"/>
+      <c r="G72" s="84"/>
+      <c r="H72" s="84"/>
+      <c r="I72" s="72"/>
+      <c r="J72" s="72"/>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A73" s="37" t="s">
+        <v>126</v>
+      </c>
+      <c r="B73" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C73" s="31" t="s">
+        <v>180</v>
+      </c>
+      <c r="D73" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="E73" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="F73" s="68" t="s">
+        <v>215</v>
+      </c>
+      <c r="G73" s="80" t="s">
+        <v>244</v>
+      </c>
+      <c r="H73" s="91" t="s">
+        <v>4</v>
+      </c>
+      <c r="I73" s="90" t="s">
+        <v>207</v>
+      </c>
+      <c r="J73" s="97" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="B74" s="36"/>
+      <c r="C74" s="36">
+        <v>5.7</v>
+      </c>
+      <c r="D74" s="70">
+        <f>C74/1000</f>
+        <v>5.7000000000000002E-3</v>
+      </c>
+      <c r="E74" s="36"/>
+      <c r="F74" s="70">
+        <v>4.2999999999999999E-4</v>
+      </c>
+      <c r="G74" s="87">
+        <f>D74/F74</f>
+        <v>13.255813953488373</v>
+      </c>
+      <c r="H74" s="87">
+        <v>500</v>
+      </c>
+      <c r="I74" s="87">
+        <v>15</v>
+      </c>
+      <c r="J74" s="100">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="23"/>
+      <c r="D75" s="69"/>
+      <c r="F75" s="69"/>
+      <c r="G75" s="84"/>
+      <c r="H75" s="84"/>
+      <c r="I75" s="72"/>
+      <c r="J75" s="72"/>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A76" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="B76" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C76" s="31" t="s">
+        <v>180</v>
+      </c>
+      <c r="D76" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="E76" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="F76" s="68" t="s">
+        <v>86</v>
+      </c>
+      <c r="G76" s="80" t="s">
+        <v>5</v>
+      </c>
+      <c r="H76" s="91" t="s">
+        <v>4</v>
+      </c>
+      <c r="I76" s="90" t="s">
+        <v>207</v>
+      </c>
+      <c r="J76" s="97" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A77" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="B77" t="s">
+        <v>52</v>
+      </c>
+      <c r="C77">
+        <f>24</f>
+        <v>24</v>
+      </c>
+      <c r="D77" s="69">
+        <f>C77/1000</f>
+        <v>2.4E-2</v>
+      </c>
+      <c r="E77">
+        <f>D77/D86</f>
+        <v>0.92407207762205446</v>
+      </c>
+      <c r="F77" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="G71" s="84"/>
-      <c r="H71" s="84"/>
-      <c r="I71" s="72"/>
-      <c r="J71" s="96"/>
-    </row>
-    <row r="72" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="B72" s="36"/>
-      <c r="C72" s="36">
-        <f>SUM(C69:C70)</f>
-        <v>8.2999999999999989</v>
-      </c>
-      <c r="D72" s="69">
-        <f t="shared" si="2"/>
-        <v>8.2999999999999984E-3</v>
-      </c>
-      <c r="E72" s="36"/>
-      <c r="F72" s="70">
-        <v>2.5600000000000001E-6</v>
-      </c>
-      <c r="G72" s="83">
-        <f>D72/F72</f>
-        <v>3242.1874999999991</v>
-      </c>
-      <c r="H72" s="83">
-        <v>904.86619540520076</v>
-      </c>
-      <c r="I72" s="75">
-        <v>0.38300309109725139</v>
-      </c>
-      <c r="J72" s="95">
-        <v>88.525164000000032</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="23"/>
-      <c r="D73" s="69"/>
-      <c r="F73" s="69"/>
-      <c r="G73" s="84"/>
-      <c r="H73" s="84"/>
-      <c r="I73" s="72"/>
-      <c r="J73" s="72"/>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A74" s="37" t="s">
-        <v>126</v>
-      </c>
-      <c r="B74" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="C74" s="31" t="s">
-        <v>180</v>
-      </c>
-      <c r="D74" s="68" t="s">
-        <v>96</v>
-      </c>
-      <c r="E74" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="F74" s="68" t="s">
-        <v>215</v>
-      </c>
-      <c r="G74" s="80" t="s">
-        <v>244</v>
-      </c>
-      <c r="H74" s="91" t="s">
-        <v>4</v>
-      </c>
-      <c r="I74" s="90" t="s">
-        <v>207</v>
-      </c>
-      <c r="J74" s="97" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="B75" s="36"/>
-      <c r="C75" s="36">
-        <v>5.7</v>
-      </c>
-      <c r="D75" s="70">
-        <f>C75/1000</f>
-        <v>5.7000000000000002E-3</v>
-      </c>
-      <c r="E75" s="36"/>
-      <c r="F75" s="70">
-        <v>4.2999999999999999E-4</v>
-      </c>
-      <c r="G75" s="87">
-        <f>D75/F75</f>
-        <v>13.255813953488373</v>
-      </c>
-      <c r="H75" s="87">
-        <v>500</v>
-      </c>
-      <c r="I75" s="87">
-        <v>15</v>
-      </c>
-      <c r="J75" s="100">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="23"/>
-      <c r="D76" s="69"/>
-      <c r="F76" s="69"/>
-      <c r="G76" s="84"/>
-      <c r="H76" s="84"/>
-      <c r="I76" s="72"/>
-      <c r="J76" s="72"/>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A77" s="30" t="s">
-        <v>168</v>
-      </c>
-      <c r="B77" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="C77" s="31" t="s">
-        <v>180</v>
-      </c>
-      <c r="D77" s="68" t="s">
-        <v>96</v>
-      </c>
-      <c r="E77" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="F77" s="68" t="s">
-        <v>86</v>
-      </c>
-      <c r="G77" s="80" t="s">
-        <v>5</v>
-      </c>
-      <c r="H77" s="91" t="s">
-        <v>4</v>
-      </c>
-      <c r="I77" s="90" t="s">
-        <v>207</v>
-      </c>
-      <c r="J77" s="97" t="s">
-        <v>206</v>
+      <c r="G77" s="84" t="s">
+        <v>23</v>
+      </c>
+      <c r="H77" s="88">
+        <v>960</v>
+      </c>
+      <c r="I77" s="79">
+        <v>130</v>
+      </c>
+      <c r="J77" s="101">
+        <v>130</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" s="33" t="s">
-        <v>128</v>
+        <v>250</v>
       </c>
       <c r="B78" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C78">
-        <f>24</f>
-        <v>24</v>
+        <f>4*0.29*1.7</f>
+        <v>1.9719999999999998</v>
       </c>
       <c r="D78" s="69">
         <f>C78/1000</f>
-        <v>2.4E-2</v>
+        <v>1.9719999999999998E-3</v>
       </c>
       <c r="E78">
-        <f>D78/D87</f>
-        <v>0.92407207762205446</v>
-      </c>
-      <c r="F78" s="69" t="s">
-        <v>23</v>
-      </c>
+        <f>D78/D86</f>
+        <v>7.5927922377945462E-2</v>
+      </c>
+      <c r="F78" s="69"/>
       <c r="G78" s="84" t="s">
         <v>23</v>
       </c>
       <c r="H78" s="88">
-        <v>960</v>
+        <v>500</v>
       </c>
       <c r="I78" s="79">
-        <v>130</v>
+        <v>15</v>
       </c>
       <c r="J78" s="101">
-        <v>130</v>
+        <v>15</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A79" s="33" t="s">
-        <v>250</v>
-      </c>
-      <c r="B79" t="s">
-        <v>48</v>
-      </c>
-      <c r="C79">
-        <f>4*0.29*1.7</f>
-        <v>1.9719999999999998</v>
-      </c>
-      <c r="D79" s="69">
-        <f>C79/1000</f>
-        <v>1.9719999999999998E-3</v>
-      </c>
-      <c r="E79">
-        <f>D79/D87</f>
-        <v>7.5927922377945462E-2</v>
-      </c>
+      <c r="A79" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="D79" s="69"/>
       <c r="F79" s="69"/>
-      <c r="G79" s="84" t="s">
+      <c r="G79" s="84"/>
+      <c r="H79" s="84"/>
+      <c r="I79" s="72"/>
+      <c r="J79" s="96"/>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A80" s="43" t="s">
+        <v>170</v>
+      </c>
+      <c r="B80" t="s">
         <v>23</v>
       </c>
-      <c r="H79" s="88">
-        <v>500</v>
-      </c>
-      <c r="I79" s="79">
-        <v>15</v>
-      </c>
-      <c r="J79" s="101">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A80" s="34" t="s">
-        <v>169</v>
+      <c r="C80" t="s">
+        <v>23</v>
       </c>
       <c r="D80" s="69"/>
-      <c r="F80" s="69"/>
-      <c r="G80" s="84"/>
-      <c r="H80" s="84"/>
-      <c r="I80" s="72"/>
-      <c r="J80" s="96"/>
+      <c r="F80" s="69">
+        <v>3.1203999999999998E-6</v>
+      </c>
+      <c r="G80" s="84">
+        <v>1401.4979818256384</v>
+      </c>
+      <c r="H80" s="88">
+        <v>925.07315570614492</v>
+      </c>
+      <c r="I80" s="79">
+        <v>121.26828892653627</v>
+      </c>
+      <c r="J80" s="101">
+        <v>121.26828892653627</v>
+      </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" s="43" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B81" t="s">
         <v>23</v>
@@ -6382,7 +6418,7 @@
       </c>
       <c r="D81" s="69"/>
       <c r="F81" s="69">
-        <v>3.1203999999999998E-6</v>
+        <v>1.52E-5</v>
       </c>
       <c r="G81" s="84">
         <v>1401.4979818256384</v>
@@ -6399,7 +6435,7 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" s="43" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B82" t="s">
         <v>23</v>
@@ -6409,7 +6445,7 @@
       </c>
       <c r="D82" s="69"/>
       <c r="F82" s="69">
-        <v>1.52E-5</v>
+        <v>3.3600000000000003E-8</v>
       </c>
       <c r="G82" s="84">
         <v>1401.4979818256384</v>
@@ -6426,7 +6462,7 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" s="43" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B83" t="s">
         <v>23</v>
@@ -6436,7 +6472,7 @@
       </c>
       <c r="D83" s="69"/>
       <c r="F83" s="69">
-        <v>3.3600000000000003E-8</v>
+        <v>1.92E-8</v>
       </c>
       <c r="G83" s="84">
         <v>1401.4979818256384</v>
@@ -6452,99 +6488,80 @@
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A84" s="43" t="s">
-        <v>173</v>
-      </c>
-      <c r="B84" t="s">
-        <v>23</v>
-      </c>
-      <c r="C84" t="s">
-        <v>23</v>
-      </c>
-      <c r="D84" s="69"/>
-      <c r="F84" s="69">
-        <v>1.92E-8</v>
-      </c>
-      <c r="G84" s="84">
+      <c r="A84" s="55" t="s">
+        <v>98</v>
+      </c>
+      <c r="B84" s="17"/>
+      <c r="C84" s="17"/>
+      <c r="D84" s="66"/>
+      <c r="E84" s="17"/>
+      <c r="F84" s="66"/>
+      <c r="G84" s="82"/>
+      <c r="H84" s="82"/>
+      <c r="I84" s="74"/>
+      <c r="J84" s="94"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A85" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="D85" s="69"/>
+      <c r="F85" s="69"/>
+      <c r="G85" s="84">
         <v>1401.4979818256384</v>
       </c>
-      <c r="H84" s="88">
+      <c r="H85" s="88">
         <v>925.07315570614492</v>
       </c>
-      <c r="I84" s="79">
+      <c r="I85" s="79">
         <v>121.26828892653627</v>
       </c>
-      <c r="J84" s="101">
+      <c r="J85" s="101">
         <v>121.26828892653627</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A85" s="55" t="s">
-        <v>98</v>
-      </c>
-      <c r="B85" s="17"/>
-      <c r="C85" s="17"/>
-      <c r="D85" s="66"/>
-      <c r="E85" s="17"/>
-      <c r="F85" s="66"/>
-      <c r="G85" s="82"/>
-      <c r="H85" s="82"/>
-      <c r="I85" s="74"/>
-      <c r="J85" s="94"/>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A86" s="43" t="s">
-        <v>174</v>
-      </c>
-      <c r="D86" s="69"/>
-      <c r="F86" s="69"/>
-      <c r="G86" s="84">
+    <row r="86" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="B86" s="36"/>
+      <c r="C86" s="36">
+        <f>SUM(C77:C78)</f>
+        <v>25.972000000000001</v>
+      </c>
+      <c r="D86" s="70">
+        <f>SUM(D77:D78)</f>
+        <v>2.5972000000000002E-2</v>
+      </c>
+      <c r="E86" s="36"/>
+      <c r="F86" s="70">
+        <f>F80+F81+F82*4+F83*4</f>
+        <v>1.8531600000000001E-5</v>
+      </c>
+      <c r="G86" s="83">
+        <f>D86/F86</f>
         <v>1401.4979818256384</v>
       </c>
-      <c r="H86" s="88">
+      <c r="H86" s="87">
+        <f>H77*$E$77+H78*$E$78</f>
         <v>925.07315570614492</v>
       </c>
-      <c r="I86" s="79">
+      <c r="I86" s="78">
+        <f>I77*$E$77+I78*$E$78</f>
         <v>121.26828892653627</v>
       </c>
-      <c r="J86" s="101">
+      <c r="J86" s="100">
+        <f>J77*$E$77+J78*$E$78</f>
         <v>121.26828892653627</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="B87" s="36"/>
-      <c r="C87" s="36">
-        <f>SUM(C78:C79)</f>
-        <v>25.972000000000001</v>
-      </c>
-      <c r="D87" s="70">
-        <f>SUM(D78:D79)</f>
-        <v>2.5972000000000002E-2</v>
-      </c>
-      <c r="E87" s="36"/>
-      <c r="F87" s="70">
-        <f>F81+F82+F83*4+F84*4</f>
-        <v>1.8531600000000001E-5</v>
-      </c>
-      <c r="G87" s="83">
-        <f>D87/F87</f>
-        <v>1401.4979818256384</v>
-      </c>
-      <c r="H87" s="87">
-        <f>H78*$E$78+H79*$E$79</f>
-        <v>925.07315570614492</v>
-      </c>
-      <c r="I87" s="78">
-        <f>I78*$E$78+I79*$E$79</f>
-        <v>121.26828892653627</v>
-      </c>
-      <c r="J87" s="100">
-        <f>J78*$E$78+J79*$E$79</f>
-        <v>121.26828892653627</v>
-      </c>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D87" s="69"/>
+      <c r="F87" s="69"/>
+      <c r="G87" s="84"/>
+      <c r="H87" s="84"/>
+      <c r="I87" s="72"/>
+      <c r="J87" s="72"/>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D88" s="69"/>
@@ -6562,7 +6579,10 @@
       <c r="I89" s="72"/>
       <c r="J89" s="72"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A90" s="47" t="s">
+        <v>41</v>
+      </c>
       <c r="D90" s="69"/>
       <c r="F90" s="69"/>
       <c r="G90" s="84"/>
@@ -6570,97 +6590,114 @@
       <c r="I90" s="72"/>
       <c r="J90" s="72"/>
     </row>
-    <row r="91" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="D91" s="69"/>
-      <c r="F91" s="69"/>
-      <c r="G91" s="84"/>
-      <c r="H91" s="84"/>
-      <c r="I91" s="72"/>
-      <c r="J91" s="72"/>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A91" s="46" t="s">
+        <v>117</v>
+      </c>
+      <c r="B91" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C91" s="31" t="s">
+        <v>180</v>
+      </c>
+      <c r="D91" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="E91" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="F91" s="68" t="s">
+        <v>86</v>
+      </c>
+      <c r="G91" s="80" t="s">
+        <v>5</v>
+      </c>
+      <c r="H91" s="91" t="s">
+        <v>4</v>
+      </c>
+      <c r="I91" s="90" t="s">
+        <v>207</v>
+      </c>
+      <c r="J91" s="97" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A92" s="46" t="s">
-        <v>117</v>
-      </c>
-      <c r="B92" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="C92" s="31" t="s">
-        <v>180</v>
-      </c>
-      <c r="D92" s="68" t="s">
-        <v>96</v>
-      </c>
-      <c r="E92" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="F92" s="68" t="s">
-        <v>86</v>
-      </c>
-      <c r="G92" s="80" t="s">
-        <v>5</v>
-      </c>
-      <c r="H92" s="91" t="s">
-        <v>4</v>
-      </c>
-      <c r="I92" s="90" t="s">
-        <v>207</v>
-      </c>
-      <c r="J92" s="97" t="s">
-        <v>206</v>
+      <c r="A92" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="C92">
+        <v>0.9</v>
+      </c>
+      <c r="D92" s="69">
+        <f>C92/1000</f>
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="E92">
+        <v>1</v>
+      </c>
+      <c r="F92" s="69">
+        <v>3.96E-7</v>
+      </c>
+      <c r="G92" s="85">
+        <f>D92/F92</f>
+        <v>2272.7272727272725</v>
+      </c>
+      <c r="H92" s="81">
+        <v>325</v>
+      </c>
+      <c r="I92" s="81">
+        <v>50</v>
+      </c>
+      <c r="J92" s="93">
+        <v>50</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A93" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="C93">
+      <c r="A93" s="55" t="s">
+        <v>98</v>
+      </c>
+      <c r="B93" s="17"/>
+      <c r="C93" s="17"/>
+      <c r="D93" s="66"/>
+      <c r="E93" s="17"/>
+      <c r="F93" s="66"/>
+      <c r="G93" s="82"/>
+      <c r="H93" s="82"/>
+      <c r="I93" s="82"/>
+      <c r="J93" s="94"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A94" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="C94">
         <v>0.9</v>
       </c>
-      <c r="D93" s="69">
-        <f>C93/1000</f>
+      <c r="D94" s="69">
+        <f>C94/1000</f>
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="E93">
+      <c r="E94">
         <v>1</v>
       </c>
-      <c r="F93" s="69">
-        <v>3.96E-7</v>
-      </c>
-      <c r="G93" s="85">
-        <f>D93/F93</f>
+      <c r="F94" s="69"/>
+      <c r="G94" s="85">
         <v>2272.7272727272725</v>
       </c>
-      <c r="H93" s="81">
+      <c r="H94" s="85">
         <v>325</v>
       </c>
-      <c r="I93" s="81">
+      <c r="I94" s="85">
         <v>50</v>
       </c>
-      <c r="J93" s="93">
+      <c r="J94" s="98">
         <v>50</v>
       </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A94" s="55" t="s">
-        <v>98</v>
-      </c>
-      <c r="B94" s="17"/>
-      <c r="C94" s="17"/>
-      <c r="D94" s="66"/>
-      <c r="E94" s="17"/>
-      <c r="F94" s="66"/>
-      <c r="G94" s="82"/>
-      <c r="H94" s="82"/>
-      <c r="I94" s="82"/>
-      <c r="J94" s="94"/>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95" s="34" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C95">
         <v>0.9</v>
@@ -6688,7 +6725,7 @@
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" s="34" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C96">
         <v>0.9</v>
@@ -6714,133 +6751,113 @@
         <v>50</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A97" s="34" t="s">
-        <v>119</v>
-      </c>
-      <c r="C97">
+    <row r="97" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="40" t="s">
+        <v>120</v>
+      </c>
+      <c r="B97" s="36"/>
+      <c r="C97" s="36">
         <v>0.9</v>
       </c>
-      <c r="D97" s="69">
+      <c r="D97" s="70">
         <f>C97/1000</f>
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="E97">
+      <c r="E97" s="36">
         <v>1</v>
       </c>
-      <c r="F97" s="69"/>
-      <c r="G97" s="85">
+      <c r="F97" s="70"/>
+      <c r="G97" s="83">
         <v>2272.7272727272725</v>
       </c>
-      <c r="H97" s="85">
+      <c r="H97" s="83">
         <v>325</v>
       </c>
-      <c r="I97" s="85">
+      <c r="I97" s="83">
         <v>50</v>
       </c>
-      <c r="J97" s="98">
+      <c r="J97" s="95">
         <v>50</v>
       </c>
     </row>
     <row r="98" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="40" t="s">
-        <v>120</v>
-      </c>
-      <c r="B98" s="36"/>
-      <c r="C98" s="36">
-        <v>0.9</v>
-      </c>
-      <c r="D98" s="70">
-        <f>C98/1000</f>
-        <v>8.9999999999999998E-4</v>
-      </c>
-      <c r="E98" s="36">
-        <v>1</v>
-      </c>
-      <c r="F98" s="70"/>
-      <c r="G98" s="83">
-        <v>2272.7272727272725</v>
-      </c>
-      <c r="H98" s="83">
-        <v>325</v>
-      </c>
-      <c r="I98" s="83">
-        <v>50</v>
-      </c>
-      <c r="J98" s="95">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D99" s="69"/>
-      <c r="F99" s="69"/>
-      <c r="G99" s="84"/>
-      <c r="H99" s="84"/>
-      <c r="I99" s="72"/>
-      <c r="J99" s="72"/>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A100" s="46" t="s">
+      <c r="D98" s="69"/>
+      <c r="F98" s="69"/>
+      <c r="G98" s="84"/>
+      <c r="H98" s="84"/>
+      <c r="I98" s="72"/>
+      <c r="J98" s="72"/>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A99" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="B100" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="C100" s="31" t="s">
+      <c r="B99" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C99" s="31" t="s">
         <v>180</v>
       </c>
-      <c r="D100" s="68" t="s">
+      <c r="D99" s="68" t="s">
         <v>96</v>
       </c>
-      <c r="E100" s="31" t="s">
+      <c r="E99" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="F100" s="68" t="s">
+      <c r="F99" s="68" t="s">
         <v>86</v>
       </c>
-      <c r="G100" s="80" t="s">
+      <c r="G99" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="H100" s="91" t="s">
+      <c r="H99" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="I100" s="90" t="s">
+      <c r="I99" s="90" t="s">
         <v>207</v>
       </c>
-      <c r="J100" s="97" t="s">
+      <c r="J99" s="97" t="s">
         <v>206</v>
       </c>
-      <c r="K100" s="22"/>
-    </row>
-    <row r="101" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="35" t="s">
+      <c r="K99" s="22"/>
+    </row>
+    <row r="100" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A100" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="B101" s="36"/>
-      <c r="C101" s="36">
+      <c r="B100" s="36"/>
+      <c r="C100" s="36">
         <v>34</v>
       </c>
-      <c r="D101" s="70">
-        <f>C101/1000</f>
+      <c r="D100" s="70">
+        <f>C100/1000</f>
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="E101" s="36"/>
-      <c r="F101" s="70">
+      <c r="E100" s="36"/>
+      <c r="F100" s="70">
         <v>1.216E-5</v>
       </c>
-      <c r="G101" s="83">
-        <f>D101/F101</f>
+      <c r="G100" s="83">
+        <f>D100/F100</f>
         <v>2796.0526315789475</v>
       </c>
-      <c r="H101" s="87">
+      <c r="H100" s="87">
         <v>1000</v>
       </c>
-      <c r="I101" s="75">
+      <c r="I100" s="75">
         <v>0.6</v>
       </c>
-      <c r="J101" s="95">
+      <c r="J100" s="95">
         <v>2.5</v>
       </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D101" s="69"/>
+      <c r="F101" s="69"/>
+      <c r="G101" s="84"/>
+      <c r="H101" s="84"/>
+      <c r="I101" s="72"/>
+      <c r="J101" s="72"/>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D102" s="69"/>
@@ -6850,198 +6867,198 @@
       <c r="I102" s="72"/>
       <c r="J102" s="72"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A103" s="13" t="s">
+        <v>53</v>
+      </c>
       <c r="D103" s="69"/>
       <c r="F103" s="69"/>
       <c r="G103" s="84"/>
       <c r="H103" s="84"/>
-      <c r="I103" s="72"/>
+      <c r="I103" s="72">
+        <v>2</v>
+      </c>
       <c r="J103" s="72"/>
     </row>
-    <row r="104" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A104" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="D104" s="69"/>
-      <c r="F104" s="69"/>
-      <c r="G104" s="84"/>
-      <c r="H104" s="84"/>
-      <c r="I104" s="72">
-        <v>2</v>
-      </c>
-      <c r="J104" s="72"/>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A104" s="48" t="s">
+        <v>124</v>
+      </c>
+      <c r="B104" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C104" s="31" t="s">
+        <v>180</v>
+      </c>
+      <c r="D104" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="E104" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="F104" s="68" t="s">
+        <v>86</v>
+      </c>
+      <c r="G104" s="80" t="s">
+        <v>5</v>
+      </c>
+      <c r="H104" s="91" t="s">
+        <v>4</v>
+      </c>
+      <c r="I104" s="90" t="s">
+        <v>207</v>
+      </c>
+      <c r="J104" s="97" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A105" s="48" t="s">
-        <v>124</v>
-      </c>
-      <c r="B105" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="C105" s="31" t="s">
-        <v>180</v>
-      </c>
-      <c r="D105" s="68" t="s">
-        <v>96</v>
-      </c>
-      <c r="E105" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="F105" s="68" t="s">
-        <v>86</v>
-      </c>
-      <c r="G105" s="80" t="s">
-        <v>5</v>
-      </c>
-      <c r="H105" s="91" t="s">
-        <v>4</v>
-      </c>
-      <c r="I105" s="90" t="s">
-        <v>207</v>
-      </c>
-      <c r="J105" s="97" t="s">
-        <v>206</v>
+      <c r="A105" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="B105" t="s">
+        <v>17</v>
+      </c>
+      <c r="C105">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="D105" s="69">
+        <f>C105/1000</f>
+        <v>3.2499999999999999E-4</v>
+      </c>
+      <c r="E105">
+        <f>D105/$D$107</f>
+        <v>0.44827586206896552</v>
+      </c>
+      <c r="F105" s="69" t="s">
+        <v>23</v>
+      </c>
+      <c r="G105" s="88">
+        <v>8800</v>
+      </c>
+      <c r="H105" s="88">
+        <v>380</v>
+      </c>
+      <c r="I105" s="79">
+        <v>62</v>
+      </c>
+      <c r="J105" s="101">
+        <v>62</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106" s="38" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B106" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C106">
-        <v>0.32500000000000001</v>
+        <v>0.4</v>
       </c>
       <c r="D106" s="69">
         <f>C106/1000</f>
-        <v>3.2499999999999999E-4</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="E106">
-        <f>D106/$D$108</f>
-        <v>0.44827586206896552</v>
+        <f>D106/$D$107</f>
+        <v>0.55172413793103459</v>
       </c>
       <c r="F106" s="69" t="s">
         <v>23</v>
       </c>
       <c r="G106" s="88">
-        <v>8800</v>
+        <v>1070</v>
       </c>
       <c r="H106" s="88">
-        <v>380</v>
+        <v>1990</v>
       </c>
       <c r="I106" s="79">
-        <v>62</v>
+        <v>0.16200000000000001</v>
       </c>
       <c r="J106" s="101">
-        <v>62</v>
+        <v>0.16200000000000001</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A107" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="B107" t="s">
-        <v>21</v>
+      <c r="A107" s="39" t="s">
+        <v>92</v>
       </c>
       <c r="C107">
-        <v>0.4</v>
+        <f>SUM(C105:C106)</f>
+        <v>0.72500000000000009</v>
       </c>
       <c r="D107" s="69">
-        <f>C107/1000</f>
-        <v>4.0000000000000002E-4</v>
+        <f>SUM(D105:D106)</f>
+        <v>7.2499999999999995E-4</v>
       </c>
       <c r="E107">
-        <f>D107/$D$108</f>
-        <v>0.55172413793103459</v>
-      </c>
-      <c r="F107" s="69" t="s">
-        <v>23</v>
-      </c>
-      <c r="G107" s="88">
-        <v>1070</v>
-      </c>
-      <c r="H107" s="88">
-        <v>1990</v>
-      </c>
-      <c r="I107" s="79">
-        <v>0.16200000000000001</v>
-      </c>
-      <c r="J107" s="101">
-        <v>0.16200000000000001</v>
+        <f>SUM(E105:E106)</f>
+        <v>1</v>
+      </c>
+      <c r="F107" s="69">
+        <v>2.8980000000000001E-7</v>
+      </c>
+      <c r="G107" s="85">
+        <f>D107/F107</f>
+        <v>2501.7253278122839</v>
+      </c>
+      <c r="H107" s="85">
+        <f>H105*$E$105+H106*$E$106</f>
+        <v>1268.2758620689658</v>
+      </c>
+      <c r="I107" s="76">
+        <f>I105*$E$105+I106*$E$106</f>
+        <v>27.882482758620689</v>
+      </c>
+      <c r="J107" s="98">
+        <f>J105*$E$105+J106*$E$106</f>
+        <v>27.882482758620689</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A108" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="C108">
-        <f>SUM(C106:C107)</f>
-        <v>0.72500000000000009</v>
-      </c>
-      <c r="D108" s="69">
-        <f>SUM(D106:D107)</f>
-        <v>7.2499999999999995E-4</v>
-      </c>
-      <c r="E108">
-        <f>SUM(E106:E107)</f>
-        <v>1</v>
-      </c>
-      <c r="F108" s="69">
-        <v>2.8980000000000001E-7</v>
-      </c>
-      <c r="G108" s="85">
-        <f>D108/F108</f>
+      <c r="A108" s="55" t="s">
+        <v>98</v>
+      </c>
+      <c r="B108" s="17"/>
+      <c r="C108" s="17"/>
+      <c r="D108" s="66"/>
+      <c r="E108" s="17"/>
+      <c r="F108" s="66"/>
+      <c r="G108" s="82"/>
+      <c r="H108" s="82"/>
+      <c r="I108" s="74"/>
+      <c r="J108" s="94"/>
+    </row>
+    <row r="109" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A109" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="B109" s="36"/>
+      <c r="C109" s="36"/>
+      <c r="D109" s="70"/>
+      <c r="E109" s="36"/>
+      <c r="F109" s="70"/>
+      <c r="G109" s="83">
         <v>2501.7253278122839</v>
       </c>
-      <c r="H108" s="85">
-        <f>H106*$E$106+H107*$E$107</f>
+      <c r="H109" s="83">
         <v>1268.2758620689658</v>
       </c>
-      <c r="I108" s="76">
-        <f>I106*$E$106+I107*$E$107</f>
+      <c r="I109" s="75">
         <v>27.882482758620689</v>
       </c>
-      <c r="J108" s="98">
-        <f>J106*$E$106+J107*$E$107</f>
+      <c r="J109" s="95">
         <v>27.882482758620689</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A109" s="55" t="s">
-        <v>98</v>
-      </c>
-      <c r="B109" s="17"/>
-      <c r="C109" s="17"/>
-      <c r="D109" s="66"/>
-      <c r="E109" s="17"/>
-      <c r="F109" s="66"/>
-      <c r="G109" s="82"/>
-      <c r="H109" s="82"/>
-      <c r="I109" s="74"/>
-      <c r="J109" s="94"/>
-    </row>
-    <row r="110" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A110" s="40" t="s">
-        <v>125</v>
-      </c>
-      <c r="B110" s="36"/>
-      <c r="C110" s="36"/>
-      <c r="D110" s="70"/>
-      <c r="E110" s="36"/>
-      <c r="F110" s="70"/>
-      <c r="G110" s="83">
-        <v>2501.7253278122839</v>
-      </c>
-      <c r="H110" s="83">
-        <v>1268.2758620689658</v>
-      </c>
-      <c r="I110" s="75">
-        <v>27.882482758620689</v>
-      </c>
-      <c r="J110" s="95">
-        <v>27.882482758620689</v>
-      </c>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D110" s="69"/>
+      <c r="F110" s="69"/>
+      <c r="G110" s="84"/>
+      <c r="H110" s="84"/>
+      <c r="I110" s="72"/>
+      <c r="J110" s="72"/>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D111" s="69"/>
@@ -7051,7 +7068,10 @@
       <c r="I111" s="72"/>
       <c r="J111" s="72"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A112" s="16" t="s">
+        <v>28</v>
+      </c>
       <c r="D112" s="69"/>
       <c r="F112" s="69"/>
       <c r="G112" s="84"/>
@@ -7059,98 +7079,120 @@
       <c r="I112" s="72"/>
       <c r="J112" s="72"/>
     </row>
-    <row r="113" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A113" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D113" s="69"/>
-      <c r="F113" s="69"/>
-      <c r="G113" s="84"/>
-      <c r="H113" s="84"/>
-      <c r="I113" s="72"/>
-      <c r="J113" s="72"/>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A113" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="B113" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C113" s="31" t="s">
+        <v>180</v>
+      </c>
+      <c r="D113" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="E113" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="F113" s="68" t="s">
+        <v>86</v>
+      </c>
+      <c r="G113" s="80" t="s">
+        <v>5</v>
+      </c>
+      <c r="H113" s="91" t="s">
+        <v>4</v>
+      </c>
+      <c r="I113" s="90" t="s">
+        <v>207</v>
+      </c>
+      <c r="J113" s="97" t="s">
+        <v>206</v>
+      </c>
+      <c r="L113" s="22"/>
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A114" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="B114" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="C114" s="31" t="s">
-        <v>180</v>
-      </c>
-      <c r="D114" s="68" t="s">
-        <v>96</v>
-      </c>
-      <c r="E114" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="F114" s="68" t="s">
-        <v>86</v>
-      </c>
-      <c r="G114" s="80" t="s">
-        <v>5</v>
-      </c>
-      <c r="H114" s="91" t="s">
-        <v>4</v>
-      </c>
-      <c r="I114" s="90" t="s">
-        <v>207</v>
-      </c>
-      <c r="J114" s="97" t="s">
-        <v>206</v>
-      </c>
-      <c r="L114" s="22"/>
+      <c r="A114" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="B114" t="s">
+        <v>51</v>
+      </c>
+      <c r="C114">
+        <v>30</v>
+      </c>
+      <c r="D114" s="69">
+        <f>C114/1000</f>
+        <v>0.03</v>
+      </c>
+      <c r="E114">
+        <v>1</v>
+      </c>
+      <c r="F114" s="69" t="s">
+        <v>23</v>
+      </c>
+      <c r="G114" s="88" t="s">
+        <v>23</v>
+      </c>
+      <c r="H114" s="88" t="s">
+        <v>23</v>
+      </c>
+      <c r="I114" s="79" t="s">
+        <v>23</v>
+      </c>
+      <c r="J114" s="96" t="s">
+        <v>23</v>
+      </c>
+      <c r="L114" s="7"/>
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A115" s="33" t="s">
-        <v>128</v>
-      </c>
-      <c r="B115" t="s">
-        <v>51</v>
-      </c>
-      <c r="C115">
-        <v>30</v>
-      </c>
-      <c r="D115" s="69">
-        <f>C115/1000</f>
-        <v>0.03</v>
-      </c>
-      <c r="E115">
-        <v>1</v>
-      </c>
-      <c r="F115" s="69" t="s">
+      <c r="A115" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="D115" s="69"/>
+      <c r="F115" s="69"/>
+      <c r="G115" s="84"/>
+      <c r="H115" s="84"/>
+      <c r="I115" s="72"/>
+      <c r="J115" s="96"/>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A116" s="49" t="s">
+        <v>131</v>
+      </c>
+      <c r="B116" t="s">
         <v>23</v>
       </c>
-      <c r="G115" s="88" t="s">
+      <c r="C116" t="s">
         <v>23</v>
       </c>
-      <c r="H115" s="88" t="s">
+      <c r="D116" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="I115" s="79" t="s">
+      <c r="E116" t="s">
         <v>23</v>
       </c>
-      <c r="J115" s="96" t="s">
-        <v>23</v>
-      </c>
-      <c r="L115" s="7"/>
-    </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A116" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="D116" s="69"/>
-      <c r="F116" s="69"/>
-      <c r="G116" s="84"/>
-      <c r="H116" s="84"/>
-      <c r="I116" s="72"/>
-      <c r="J116" s="96"/>
+      <c r="F116" s="69">
+        <v>2.6599999999999999E-6</v>
+      </c>
+      <c r="G116" s="85">
+        <f>$G$128</f>
+        <v>1885.8436007040482</v>
+      </c>
+      <c r="H116" s="81">
+        <v>1010</v>
+      </c>
+      <c r="I116" s="73">
+        <v>0.27</v>
+      </c>
+      <c r="J116" s="93">
+        <v>0.27</v>
+      </c>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A117" s="49" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B117" t="s">
         <v>23</v>
@@ -7165,10 +7207,10 @@
         <v>23</v>
       </c>
       <c r="F117" s="69">
-        <v>2.6599999999999999E-6</v>
+        <v>7.9800000000000003E-7</v>
       </c>
       <c r="G117" s="85">
-        <f>$G$129</f>
+        <f t="shared" ref="G117:G121" si="3">$G$128</f>
         <v>1885.8436007040482</v>
       </c>
       <c r="H117" s="81">
@@ -7183,7 +7225,7 @@
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A118" s="49" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B118" t="s">
         <v>23</v>
@@ -7201,7 +7243,7 @@
         <v>7.9800000000000003E-7</v>
       </c>
       <c r="G118" s="85">
-        <f t="shared" ref="G118:G122" si="3">$G$129</f>
+        <f t="shared" si="3"/>
         <v>1885.8436007040482</v>
       </c>
       <c r="H118" s="81">
@@ -7216,7 +7258,7 @@
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A119" s="49" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B119" t="s">
         <v>23</v>
@@ -7231,7 +7273,7 @@
         <v>23</v>
       </c>
       <c r="F119" s="69">
-        <v>7.9800000000000003E-7</v>
+        <v>2.9440000000000001E-6</v>
       </c>
       <c r="G119" s="85">
         <f t="shared" si="3"/>
@@ -7249,7 +7291,7 @@
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A120" s="49" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B120" t="s">
         <v>23</v>
@@ -7282,7 +7324,7 @@
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A121" s="49" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="B121" t="s">
         <v>23</v>
@@ -7297,7 +7339,7 @@
         <v>23</v>
       </c>
       <c r="F121" s="69">
-        <v>2.9440000000000001E-6</v>
+        <v>5.2440000000000001E-6</v>
       </c>
       <c r="G121" s="85">
         <f t="shared" si="3"/>
@@ -7314,91 +7356,83 @@
       </c>
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A122" s="49" t="s">
-        <v>135</v>
+      <c r="A122" s="56" t="s">
+        <v>252</v>
       </c>
       <c r="B122" t="s">
         <v>23</v>
       </c>
-      <c r="C122" t="s">
-        <v>23</v>
-      </c>
-      <c r="D122" s="69" t="s">
-        <v>23</v>
-      </c>
-      <c r="E122" t="s">
-        <v>23</v>
+      <c r="C122">
+        <f>SUM(C123:C124)</f>
+        <v>0.30199515966809148</v>
+      </c>
+      <c r="D122" s="69">
+        <f>SUM(D123:D124)</f>
+        <v>3.0199515966809152E-4</v>
+      </c>
+      <c r="E122">
+        <v>1</v>
       </c>
       <c r="F122" s="69">
-        <v>5.2440000000000001E-6</v>
+        <v>1.3E-7</v>
       </c>
       <c r="G122" s="85">
-        <f t="shared" si="3"/>
-        <v>1885.8436007040482</v>
+        <f>(1.7*0.1775/1000)/F122+G121</f>
+        <v>4206.9974468578948</v>
       </c>
       <c r="H122" s="81">
-        <v>1010</v>
-      </c>
-      <c r="I122" s="73">
-        <v>0.27</v>
+        <v>500</v>
+      </c>
+      <c r="I122" s="81">
+        <v>15</v>
       </c>
       <c r="J122" s="93">
-        <v>0.27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A123" s="56" t="s">
-        <v>252</v>
+      <c r="A123" s="57" t="s">
+        <v>51</v>
       </c>
       <c r="B123" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="C123">
-        <f>SUM(C124:C125)</f>
-        <v>0.30199515966809148</v>
+        <f>F122*G121</f>
+        <v>2.4515966809152628E-4</v>
       </c>
       <c r="D123" s="69">
-        <f>SUM(D124:D125)</f>
-        <v>3.0199515966809152E-4</v>
+        <f>C123/1000</f>
+        <v>2.4515966809152627E-7</v>
       </c>
       <c r="E123">
-        <v>1</v>
-      </c>
-      <c r="F123" s="69">
-        <v>1.3E-7</v>
-      </c>
-      <c r="G123" s="85">
-        <f>(1.7*0.1775/1000)/F123+G122</f>
-        <v>4206.9974468578948</v>
-      </c>
-      <c r="H123" s="81">
-        <v>500</v>
-      </c>
-      <c r="I123" s="81">
-        <v>15</v>
-      </c>
-      <c r="J123" s="93">
-        <v>15</v>
-      </c>
+        <f>D123/D122</f>
+        <v>8.1179999163221545E-4</v>
+      </c>
+      <c r="F123" s="69"/>
+      <c r="G123" s="89"/>
+      <c r="H123" s="92"/>
+      <c r="I123" s="92"/>
+      <c r="J123" s="102"/>
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A124" s="57" t="s">
-        <v>51</v>
+      <c r="A124" s="49" t="s">
+        <v>255</v>
       </c>
       <c r="B124" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C124">
-        <f>F123*G122</f>
-        <v>2.4515966809152628E-4</v>
+        <f>1.7*0.1775</f>
+        <v>0.30174999999999996</v>
       </c>
       <c r="D124" s="69">
         <f>C124/1000</f>
-        <v>2.4515966809152627E-7</v>
+        <v>3.0174999999999999E-4</v>
       </c>
       <c r="E124">
-        <f>D124/D123</f>
-        <v>8.1179999163221545E-4</v>
+        <f>D124/D122</f>
+        <v>0.99918820000836783</v>
       </c>
       <c r="F124" s="69"/>
       <c r="G124" s="89"/>
@@ -7408,32 +7442,39 @@
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A125" s="49" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B125" t="s">
-        <v>48</v>
-      </c>
-      <c r="C125">
-        <f>1.7*0.1775</f>
-        <v>0.30174999999999996</v>
-      </c>
-      <c r="D125" s="69">
-        <f>C125/1000</f>
-        <v>3.0174999999999999E-4</v>
-      </c>
-      <c r="E125">
-        <f>D125/D123</f>
-        <v>0.99918820000836783</v>
-      </c>
-      <c r="F125" s="69"/>
-      <c r="G125" s="89"/>
-      <c r="H125" s="92"/>
-      <c r="I125" s="92"/>
-      <c r="J125" s="102"/>
+        <v>23</v>
+      </c>
+      <c r="C125" t="s">
+        <v>23</v>
+      </c>
+      <c r="D125" s="69" t="s">
+        <v>23</v>
+      </c>
+      <c r="E125" t="s">
+        <v>23</v>
+      </c>
+      <c r="F125" s="69">
+        <v>1.3E-7</v>
+      </c>
+      <c r="G125" s="85">
+        <v>4206.9974468578948</v>
+      </c>
+      <c r="H125" s="81">
+        <v>500</v>
+      </c>
+      <c r="I125" s="81">
+        <v>15</v>
+      </c>
+      <c r="J125" s="93">
+        <v>15</v>
+      </c>
     </row>
     <row r="126" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A126" s="49" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="B126" t="s">
         <v>23</v>
@@ -7465,7 +7506,7 @@
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A127" s="49" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B127" t="s">
         <v>23</v>
@@ -7495,134 +7536,136 @@
         <v>15</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A128" s="49" t="s">
-        <v>253</v>
-      </c>
-      <c r="B128" t="s">
-        <v>23</v>
-      </c>
-      <c r="C128" t="s">
-        <v>23</v>
-      </c>
-      <c r="D128" s="69" t="s">
-        <v>23</v>
-      </c>
-      <c r="E128" t="s">
-        <v>23</v>
-      </c>
-      <c r="F128" s="69">
-        <v>1.3E-7</v>
-      </c>
-      <c r="G128" s="85">
-        <v>4206.9974468578948</v>
-      </c>
-      <c r="H128" s="81">
-        <v>500</v>
-      </c>
-      <c r="I128" s="81">
-        <v>15</v>
-      </c>
-      <c r="J128" s="93">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="129" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A129" s="35" t="s">
+    <row r="128" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A128" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="B129" s="36"/>
-      <c r="C129" s="36"/>
-      <c r="D129" s="70"/>
-      <c r="E129" s="36"/>
-      <c r="F129" s="70">
-        <f>SUM(F117:F128)</f>
+      <c r="B128" s="36"/>
+      <c r="C128" s="36"/>
+      <c r="D128" s="70"/>
+      <c r="E128" s="36"/>
+      <c r="F128" s="70">
+        <f>SUM(F116:F127)</f>
         <v>1.5908000000000001E-5</v>
       </c>
-      <c r="G129" s="83">
-        <f>D115/F129</f>
+      <c r="G128" s="83">
+        <f>D114/F128</f>
         <v>1885.8436007040482</v>
       </c>
-      <c r="H129" s="87">
+      <c r="H128" s="87">
         <v>1010</v>
       </c>
-      <c r="I129" s="78">
+      <c r="I128" s="78">
         <v>0.27</v>
       </c>
-      <c r="J129" s="100">
+      <c r="J128" s="100">
         <v>0.27</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A130" s="3"/>
-      <c r="C130" s="3"/>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A129" s="3"/>
+      <c r="C129" s="3"/>
+      <c r="D129" s="69"/>
+      <c r="F129" s="69"/>
+      <c r="H129" s="84"/>
+      <c r="I129" s="72"/>
+      <c r="J129" s="72"/>
+    </row>
+    <row r="130" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A130" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="D130" s="69"/>
-      <c r="F130" s="69"/>
+      <c r="F130" s="71"/>
       <c r="H130" s="84"/>
       <c r="I130" s="72"/>
       <c r="J130" s="72"/>
     </row>
-    <row r="131" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A131" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D131" s="69"/>
-      <c r="F131" s="71"/>
-      <c r="H131" s="84"/>
-      <c r="I131" s="72"/>
-      <c r="J131" s="72"/>
+    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A131" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="B131" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C131" s="31" t="s">
+        <v>180</v>
+      </c>
+      <c r="D131" s="68" t="s">
+        <v>96</v>
+      </c>
+      <c r="E131" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="F131" s="68" t="s">
+        <v>86</v>
+      </c>
+      <c r="G131" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="H131" s="91" t="s">
+        <v>4</v>
+      </c>
+      <c r="I131" s="90" t="s">
+        <v>207</v>
+      </c>
+      <c r="J131" s="97" t="s">
+        <v>206</v>
+      </c>
+      <c r="L131" s="22"/>
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A132" s="48" t="s">
-        <v>175</v>
-      </c>
-      <c r="B132" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="C132" s="31" t="s">
-        <v>180</v>
-      </c>
-      <c r="D132" s="68" t="s">
-        <v>96</v>
-      </c>
-      <c r="E132" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="F132" s="68" t="s">
-        <v>86</v>
-      </c>
-      <c r="G132" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="H132" s="91" t="s">
-        <v>4</v>
-      </c>
-      <c r="I132" s="90" t="s">
-        <v>207</v>
-      </c>
-      <c r="J132" s="97" t="s">
-        <v>206</v>
-      </c>
-      <c r="L132" s="22"/>
+      <c r="A132" s="38" t="s">
+        <v>176</v>
+      </c>
+      <c r="B132" t="s">
+        <v>48</v>
+      </c>
+      <c r="C132">
+        <f>1.7*0.1775</f>
+        <v>0.30174999999999996</v>
+      </c>
+      <c r="D132" s="69">
+        <f>C132/1000</f>
+        <v>3.0174999999999999E-4</v>
+      </c>
+      <c r="E132">
+        <f>D132/$D$135</f>
+        <v>0.50992817912970001</v>
+      </c>
+      <c r="F132" s="69" t="s">
+        <v>23</v>
+      </c>
+      <c r="G132" t="s">
+        <v>23</v>
+      </c>
+      <c r="H132" s="88">
+        <v>500</v>
+      </c>
+      <c r="I132" s="88">
+        <v>15</v>
+      </c>
+      <c r="J132" s="101">
+        <v>15</v>
+      </c>
     </row>
     <row r="133" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A133" s="38" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B133" t="s">
         <v>48</v>
       </c>
       <c r="C133">
-        <f>1.7*0.1775</f>
-        <v>0.30174999999999996</v>
+        <v>0.22</v>
       </c>
       <c r="D133" s="69">
-        <f>C133/1000</f>
-        <v>3.0174999999999999E-4</v>
+        <f t="shared" ref="D133:D135" si="4">C133/1000</f>
+        <v>2.2000000000000001E-4</v>
       </c>
       <c r="E133">
-        <f>D133/$D$136</f>
-        <v>0.50992817912970001</v>
+        <f t="shared" ref="E133:E134" si="5">D133/$D$135</f>
+        <v>0.37177862272919304</v>
       </c>
       <c r="F133" s="69" t="s">
         <v>23</v>
@@ -7641,22 +7684,22 @@
       </c>
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A134" s="38" t="s">
-        <v>177</v>
+      <c r="A134" s="45" t="s">
+        <v>178</v>
       </c>
       <c r="B134" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C134">
-        <v>0.22</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="D134" s="69">
-        <f t="shared" ref="D134:D136" si="4">C134/1000</f>
-        <v>2.2000000000000001E-4</v>
+        <f t="shared" si="4"/>
+        <v>7.0000000000000007E-5</v>
       </c>
       <c r="E134">
-        <f t="shared" ref="E134:E135" si="5">D134/$D$136</f>
-        <v>0.37177862272919304</v>
+        <f t="shared" si="5"/>
+        <v>0.11829319814110689</v>
       </c>
       <c r="F134" s="69" t="s">
         <v>23</v>
@@ -7665,124 +7708,90 @@
         <v>23</v>
       </c>
       <c r="H134" s="88">
-        <v>500</v>
+        <v>900</v>
       </c>
       <c r="I134" s="88">
-        <v>15</v>
+        <v>209</v>
       </c>
       <c r="J134" s="101">
-        <v>15</v>
+        <v>209</v>
       </c>
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A135" s="45" t="s">
-        <v>178</v>
+      <c r="A135" s="39" t="s">
+        <v>92</v>
       </c>
       <c r="B135" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="C135">
-        <v>7.0000000000000007E-2</v>
+        <f>SUM(C132:C134)</f>
+        <v>0.59175</v>
       </c>
       <c r="D135" s="69">
         <f t="shared" si="4"/>
-        <v>7.0000000000000007E-5</v>
+        <v>5.9175000000000005E-4</v>
       </c>
       <c r="E135">
-        <f t="shared" si="5"/>
-        <v>0.11829319814110689</v>
-      </c>
-      <c r="F135" s="69" t="s">
-        <v>23</v>
-      </c>
-      <c r="G135" t="s">
-        <v>23</v>
-      </c>
-      <c r="H135" s="88">
-        <v>900</v>
-      </c>
-      <c r="I135" s="88">
-        <v>209</v>
-      </c>
-      <c r="J135" s="101">
-        <v>209</v>
+        <f>SUM(E132:E134)</f>
+        <v>1</v>
+      </c>
+      <c r="F135" s="69">
+        <v>1.3E-7</v>
+      </c>
+      <c r="G135" s="85">
+        <f>D135/F135</f>
+        <v>4551.9230769230771</v>
+      </c>
+      <c r="H135" s="85">
+        <f>H132*$E$132+H133*$E$133+H134*$E$134</f>
+        <v>547.3172792564427</v>
+      </c>
+      <c r="I135" s="85">
+        <v>15</v>
+      </c>
+      <c r="J135" s="98">
+        <v>15</v>
       </c>
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A136" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="B136" t="s">
-        <v>22</v>
-      </c>
-      <c r="C136">
-        <f>SUM(C133:C135)</f>
-        <v>0.59175</v>
-      </c>
-      <c r="D136" s="69">
-        <f t="shared" si="4"/>
-        <v>5.9175000000000005E-4</v>
-      </c>
-      <c r="E136">
-        <f>SUM(E133:E135)</f>
-        <v>1</v>
-      </c>
-      <c r="F136" s="69">
-        <v>1.3E-7</v>
-      </c>
-      <c r="G136" s="85">
-        <f>D136/F136</f>
+      <c r="A136" s="55" t="s">
+        <v>98</v>
+      </c>
+      <c r="B136" s="17"/>
+      <c r="C136" s="17"/>
+      <c r="D136" s="66"/>
+      <c r="E136" s="17"/>
+      <c r="F136" s="66"/>
+      <c r="G136" s="17"/>
+      <c r="H136" s="82"/>
+      <c r="I136" s="82"/>
+      <c r="J136" s="94"/>
+    </row>
+    <row r="137" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A137" s="50" t="s">
+        <v>179</v>
+      </c>
+      <c r="B137" s="36"/>
+      <c r="C137" s="36"/>
+      <c r="D137" s="70"/>
+      <c r="E137" s="36"/>
+      <c r="F137" s="70"/>
+      <c r="G137" s="83">
         <v>4551.9230769230771</v>
       </c>
-      <c r="H136" s="85">
-        <f>H133*$E$133+H134*$E$134+H135*$E$135</f>
+      <c r="H137" s="83">
         <v>547.3172792564427</v>
       </c>
-      <c r="I136" s="85">
+      <c r="I137" s="83">
         <v>15</v>
       </c>
-      <c r="J136" s="98">
+      <c r="J137" s="95">
         <v>15</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A137" s="55" t="s">
-        <v>98</v>
-      </c>
-      <c r="B137" s="17"/>
-      <c r="C137" s="17"/>
-      <c r="D137" s="66"/>
-      <c r="E137" s="17"/>
-      <c r="F137" s="66"/>
-      <c r="G137" s="17"/>
-      <c r="H137" s="82"/>
-      <c r="I137" s="82"/>
-      <c r="J137" s="94"/>
-    </row>
-    <row r="138" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A138" s="50" t="s">
-        <v>179</v>
-      </c>
-      <c r="B138" s="36"/>
-      <c r="C138" s="36"/>
-      <c r="D138" s="70"/>
-      <c r="E138" s="36"/>
-      <c r="F138" s="70"/>
-      <c r="G138" s="83">
-        <v>4551.9230769230771</v>
-      </c>
-      <c r="H138" s="83">
-        <v>547.3172792564427</v>
-      </c>
-      <c r="I138" s="83">
-        <v>15</v>
-      </c>
-      <c r="J138" s="95">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="J139" s="72"/>
+    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J138" s="72"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7844,10 +7853,10 @@
       <c r="J1" s="58" t="s">
         <v>283</v>
       </c>
-      <c r="L1" s="108" t="s">
+      <c r="L1" s="109" t="s">
         <v>377</v>
       </c>
-      <c r="M1" s="108"/>
+      <c r="M1" s="109"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -8286,7 +8295,7 @@
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="L14" s="109" t="s">
+      <c r="L14" s="110" t="s">
         <v>376</v>
       </c>
       <c r="M14" s="64"/>
@@ -8325,7 +8334,7 @@
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="L15" s="109"/>
+      <c r="L15" s="110"/>
     </row>
     <row r="16" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
@@ -9230,18 +9239,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C1" s="110" t="s">
+      <c r="C1" s="111" t="s">
         <v>384</v>
       </c>
-      <c r="D1" s="110"/>
-      <c r="E1" s="110"/>
-      <c r="F1" s="110"/>
-      <c r="H1" s="110" t="s">
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
+      <c r="F1" s="111"/>
+      <c r="H1" s="111" t="s">
         <v>383</v>
       </c>
-      <c r="I1" s="110"/>
-      <c r="J1" s="110"/>
-      <c r="K1" s="110"/>
+      <c r="I1" s="111"/>
+      <c r="J1" s="111"/>
+      <c r="K1" s="111"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">

</xml_diff>